<commit_message>
started cleaning Santa Maria data and changed disp_event ids from all areas
</commit_message>
<xml_diff>
--- a/Data/Seed_dispersal/Raw_SuzanoAnne_07d-04-2021_Seed-dispersal.xlsx
+++ b/Data/Seed_dispersal/Raw_SuzanoAnne_07d-04-2021_Seed-dispersal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Documentos\github\BLT_IBM-Model\Data\Seed_dispersal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C3CDE8-6D32-481A-BBD7-624CB539E71C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C4C7FC-F896-4175-82F8-2EBF32F289C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,511 +64,511 @@
     <t>Xylopia brasiliensis</t>
   </si>
   <si>
-    <t>SDSep1</t>
-  </si>
-  <si>
     <t>FSSep2</t>
   </si>
   <si>
-    <t>SDSep2</t>
-  </si>
-  <si>
     <t>Myrciaria cuspidata</t>
   </si>
   <si>
-    <t>SDSep3</t>
-  </si>
-  <si>
-    <t>SDSep4</t>
-  </si>
-  <si>
     <t>Trichilia catigua</t>
   </si>
   <si>
-    <t>SDSep5</t>
-  </si>
-  <si>
-    <t>SDSep6</t>
-  </si>
-  <si>
     <t>FSSep3</t>
   </si>
   <si>
     <t>Neomitranthes obscura</t>
   </si>
   <si>
-    <t>SDSep7</t>
-  </si>
-  <si>
     <t>FSSep4</t>
   </si>
   <si>
-    <t>SDSep8</t>
-  </si>
-  <si>
     <t>FSSep5</t>
   </si>
   <si>
-    <t>SDSep9</t>
-  </si>
-  <si>
     <t>FSSep6</t>
   </si>
   <si>
-    <t>SDSep10</t>
-  </si>
-  <si>
     <t>FSSep7</t>
   </si>
   <si>
-    <t>SDSep11</t>
-  </si>
-  <si>
     <t>FSSep8</t>
   </si>
   <si>
     <t>Chrysophyllum gonocarpum</t>
   </si>
   <si>
-    <t>SDSep12</t>
-  </si>
-  <si>
     <t>FSSep9</t>
   </si>
   <si>
     <t>Cordia sellowiana</t>
   </si>
   <si>
-    <t>SDSep13</t>
-  </si>
-  <si>
     <t>FSSep10</t>
   </si>
   <si>
     <t>Philodendron spp.</t>
   </si>
   <si>
-    <t>SDSep14</t>
-  </si>
-  <si>
     <t>&gt;100</t>
   </si>
   <si>
     <t>Pera glabrata</t>
   </si>
   <si>
-    <t>SDSep15</t>
-  </si>
-  <si>
     <t>FSSep11</t>
   </si>
   <si>
-    <t>SDSep16</t>
-  </si>
-  <si>
     <t>Randia armata</t>
   </si>
   <si>
-    <t>SDSep17</t>
-  </si>
-  <si>
     <t>FSSep12</t>
   </si>
   <si>
-    <t>SDSep18</t>
-  </si>
-  <si>
     <t>FSSep13</t>
   </si>
   <si>
-    <t>SDSep19</t>
-  </si>
-  <si>
     <t>FSSep14</t>
   </si>
   <si>
-    <t>SDSep20</t>
-  </si>
-  <si>
     <t>FSSep15</t>
   </si>
   <si>
     <t>Myrsine umbellata</t>
   </si>
   <si>
-    <t>SDSep21</t>
-  </si>
-  <si>
     <t>FSSep16</t>
   </si>
   <si>
-    <t>SDSep22</t>
-  </si>
-  <si>
-    <t>SDSep23</t>
-  </si>
-  <si>
-    <t>SDSep24</t>
-  </si>
-  <si>
     <t>FSDec17</t>
   </si>
   <si>
-    <t>SDDec25</t>
-  </si>
-  <si>
     <t>FSDec18</t>
   </si>
   <si>
-    <t>SDDec26</t>
-  </si>
-  <si>
     <t>FSDec19</t>
   </si>
   <si>
-    <t>SDDec27</t>
-  </si>
-  <si>
     <t>FSDec20</t>
   </si>
   <si>
-    <t>SDDec28</t>
-  </si>
-  <si>
-    <t>SDDec29</t>
-  </si>
-  <si>
     <t>FSDec21</t>
   </si>
   <si>
-    <t>SDDec30</t>
-  </si>
-  <si>
     <t>FSDec22</t>
   </si>
   <si>
-    <t>SDDec31</t>
-  </si>
-  <si>
     <t>FSDec23</t>
   </si>
   <si>
-    <t>SDDec32</t>
-  </si>
-  <si>
     <t>Rhipsalis teres</t>
   </si>
   <si>
-    <t>SDDec33</t>
-  </si>
-  <si>
-    <t>SDDec34</t>
-  </si>
-  <si>
-    <t>SDDec35</t>
-  </si>
-  <si>
     <t>FSDec24</t>
   </si>
   <si>
-    <t>SDDec36</t>
-  </si>
-  <si>
     <t>FSDec25</t>
   </si>
   <si>
-    <t>SDDec37</t>
-  </si>
-  <si>
     <t>FSDec26</t>
   </si>
   <si>
-    <t>SDDec38</t>
-  </si>
-  <si>
     <t>FSDec27</t>
   </si>
   <si>
-    <t>SDDec39</t>
-  </si>
-  <si>
     <t>FSDec28</t>
   </si>
   <si>
-    <t>SDDec40</t>
-  </si>
-  <si>
     <t>FSDec29</t>
   </si>
   <si>
-    <t>SDDec41</t>
-  </si>
-  <si>
-    <t>SDDec42</t>
-  </si>
-  <si>
     <t>FSDec30</t>
   </si>
   <si>
     <t>Casearia decandra</t>
   </si>
   <si>
-    <t>SDDec43</t>
-  </si>
-  <si>
     <t>FSDec31</t>
   </si>
   <si>
-    <t>SDDec44</t>
-  </si>
-  <si>
     <t>FSDec32</t>
   </si>
   <si>
-    <t>SDDec45</t>
-  </si>
-  <si>
     <t>FSDec33</t>
   </si>
   <si>
-    <t>SDDec46</t>
-  </si>
-  <si>
-    <t>SDDec47</t>
-  </si>
-  <si>
-    <t>SDDec48</t>
-  </si>
-  <si>
     <t>FSDec34</t>
   </si>
   <si>
-    <t>SDDec49</t>
-  </si>
-  <si>
     <t>FSDec35</t>
   </si>
   <si>
-    <t>SDDec50</t>
-  </si>
-  <si>
     <t>FSDec36</t>
   </si>
   <si>
-    <t>SDDec51</t>
-  </si>
-  <si>
-    <t>SDDec52</t>
-  </si>
-  <si>
     <t>FSDec37</t>
   </si>
   <si>
-    <t>SDDec53</t>
-  </si>
-  <si>
-    <t>SDDec54</t>
-  </si>
-  <si>
     <t>FSDec38</t>
   </si>
   <si>
-    <t>SDDec55</t>
-  </si>
-  <si>
-    <t>SDDec56</t>
-  </si>
-  <si>
     <t>FSFev39</t>
   </si>
   <si>
     <t>Campomanesia guaviroba</t>
   </si>
   <si>
-    <t>SDFev57</t>
-  </si>
-  <si>
     <t>FSFev40</t>
   </si>
   <si>
-    <t>SDFev58</t>
-  </si>
-  <si>
     <t>Celtis iguanaea</t>
   </si>
   <si>
-    <t>SDFev59</t>
-  </si>
-  <si>
-    <t>SDFev60</t>
-  </si>
-  <si>
     <t>FSFev41</t>
   </si>
   <si>
-    <t>SDFev61</t>
-  </si>
-  <si>
     <t>FSFev42</t>
   </si>
   <si>
-    <t>SDFev62</t>
-  </si>
-  <si>
     <t>FSFev43</t>
   </si>
   <si>
-    <t>SDFev63</t>
-  </si>
-  <si>
     <t>FSFev44</t>
   </si>
   <si>
     <t>Rhamnidium elaeocarpum</t>
   </si>
   <si>
-    <t>SDFev64</t>
-  </si>
-  <si>
     <t>FSFev45</t>
   </si>
   <si>
-    <t>SDFev65</t>
-  </si>
-  <si>
     <t>Sorocea bonplandii</t>
   </si>
   <si>
-    <t>SDFev66</t>
-  </si>
-  <si>
-    <t>SDFev67</t>
-  </si>
-  <si>
     <t>FSFev46</t>
   </si>
   <si>
-    <t>SDFev68</t>
-  </si>
-  <si>
-    <t>SDFev69</t>
-  </si>
-  <si>
     <t>FSFev47</t>
   </si>
   <si>
     <t>Ficus luschnathiana</t>
   </si>
   <si>
-    <t>SDFev70</t>
-  </si>
-  <si>
     <t>FSFev48</t>
   </si>
   <si>
-    <t>SDFev71</t>
-  </si>
-  <si>
-    <t>SDFev72</t>
-  </si>
-  <si>
     <t>FSFev49</t>
   </si>
   <si>
-    <t>SDFev73</t>
-  </si>
-  <si>
     <t>FSFev50</t>
   </si>
   <si>
     <t>Plinia rivularis</t>
   </si>
   <si>
-    <t>SDFev74</t>
-  </si>
-  <si>
-    <t>SDFev75</t>
-  </si>
-  <si>
     <t>FSFev51</t>
   </si>
   <si>
-    <t>SDFev76</t>
-  </si>
-  <si>
     <t>FSFev52</t>
   </si>
   <si>
-    <t>SDFev77</t>
-  </si>
-  <si>
-    <t>SDFev78</t>
-  </si>
-  <si>
     <t>FSApr53</t>
   </si>
   <si>
     <t>Cordia ecalyculata</t>
   </si>
   <si>
-    <t>SDApr79</t>
-  </si>
-  <si>
     <t>FSApr54</t>
   </si>
   <si>
-    <t>SDApr80</t>
-  </si>
-  <si>
     <t>FSApr55</t>
   </si>
   <si>
     <t>Tapirira guianensis</t>
   </si>
   <si>
-    <t>SDApr81</t>
-  </si>
-  <si>
     <t>Ficus guaranitica</t>
   </si>
   <si>
-    <t>SDApr82</t>
-  </si>
-  <si>
     <t>FSApr56</t>
   </si>
   <si>
-    <t>SDApr83</t>
-  </si>
-  <si>
     <t>FSApr57</t>
   </si>
   <si>
-    <t>SDApr84</t>
-  </si>
-  <si>
-    <t>SDApr85</t>
-  </si>
-  <si>
     <t>FSApr58</t>
   </si>
   <si>
     <t>Inga marginata</t>
   </si>
   <si>
-    <t>SDApr86</t>
-  </si>
-  <si>
     <t>Pereskia aculeata</t>
   </si>
   <si>
-    <t>SDApr87</t>
-  </si>
-  <si>
     <t>FSApr59</t>
   </si>
   <si>
-    <t>SDApr88</t>
+    <t>SDSuzSep1</t>
+  </si>
+  <si>
+    <t>SDSuzSep2</t>
+  </si>
+  <si>
+    <t>SDSuzSep3</t>
+  </si>
+  <si>
+    <t>SDSuzSep4</t>
+  </si>
+  <si>
+    <t>SDSuzSep5</t>
+  </si>
+  <si>
+    <t>SDSuzSep6</t>
+  </si>
+  <si>
+    <t>SDSuzSep7</t>
+  </si>
+  <si>
+    <t>SDSuzSep8</t>
+  </si>
+  <si>
+    <t>SDSuzSep9</t>
+  </si>
+  <si>
+    <t>SDSuzSep10</t>
+  </si>
+  <si>
+    <t>SDSuzSep11</t>
+  </si>
+  <si>
+    <t>SDSuzSep12</t>
+  </si>
+  <si>
+    <t>SDSuzSep13</t>
+  </si>
+  <si>
+    <t>SDSuzSep14</t>
+  </si>
+  <si>
+    <t>SDSuzSep15</t>
+  </si>
+  <si>
+    <t>SDSuzSep16</t>
+  </si>
+  <si>
+    <t>SDSuzSep17</t>
+  </si>
+  <si>
+    <t>SDSuzSep18</t>
+  </si>
+  <si>
+    <t>SDSuzSep19</t>
+  </si>
+  <si>
+    <t>SDSuzSep20</t>
+  </si>
+  <si>
+    <t>SDSuzSep21</t>
+  </si>
+  <si>
+    <t>SDSuzSep22</t>
+  </si>
+  <si>
+    <t>SDSuzSep23</t>
+  </si>
+  <si>
+    <t>SDSuzSep24</t>
+  </si>
+  <si>
+    <t>SDSuzDec25</t>
+  </si>
+  <si>
+    <t>SDSuzDec26</t>
+  </si>
+  <si>
+    <t>SDSuzDec27</t>
+  </si>
+  <si>
+    <t>SDSuzDec28</t>
+  </si>
+  <si>
+    <t>SDSuzDec29</t>
+  </si>
+  <si>
+    <t>SDSuzDec30</t>
+  </si>
+  <si>
+    <t>SDSuzDec31</t>
+  </si>
+  <si>
+    <t>SDSuzDec32</t>
+  </si>
+  <si>
+    <t>SDSuzDec33</t>
+  </si>
+  <si>
+    <t>SDSuzDec34</t>
+  </si>
+  <si>
+    <t>SDSuzDec35</t>
+  </si>
+  <si>
+    <t>SDSuzDec36</t>
+  </si>
+  <si>
+    <t>SDSuzDec37</t>
+  </si>
+  <si>
+    <t>SDSuzDec38</t>
+  </si>
+  <si>
+    <t>SDSuzDec39</t>
+  </si>
+  <si>
+    <t>SDSuzDec40</t>
+  </si>
+  <si>
+    <t>SDSuzDec41</t>
+  </si>
+  <si>
+    <t>SDSuzDec42</t>
+  </si>
+  <si>
+    <t>SDSuzDec43</t>
+  </si>
+  <si>
+    <t>SDSuzDec44</t>
+  </si>
+  <si>
+    <t>SDSuzDec45</t>
+  </si>
+  <si>
+    <t>SDSuzDec46</t>
+  </si>
+  <si>
+    <t>SDSuzDec47</t>
+  </si>
+  <si>
+    <t>SDSuzDec48</t>
+  </si>
+  <si>
+    <t>SDSuzDec49</t>
+  </si>
+  <si>
+    <t>SDSuzDec50</t>
+  </si>
+  <si>
+    <t>SDSuzDec51</t>
+  </si>
+  <si>
+    <t>SDSuzDec52</t>
+  </si>
+  <si>
+    <t>SDSuzDec53</t>
+  </si>
+  <si>
+    <t>SDSuzDec54</t>
+  </si>
+  <si>
+    <t>SDSuzDec55</t>
+  </si>
+  <si>
+    <t>SDSuzDec56</t>
+  </si>
+  <si>
+    <t>SDSuzFev57</t>
+  </si>
+  <si>
+    <t>SDSuzFev58</t>
+  </si>
+  <si>
+    <t>SDSuzFev59</t>
+  </si>
+  <si>
+    <t>SDSuzFev60</t>
+  </si>
+  <si>
+    <t>SDSuzFev61</t>
+  </si>
+  <si>
+    <t>SDSuzFev62</t>
+  </si>
+  <si>
+    <t>SDSuzFev63</t>
+  </si>
+  <si>
+    <t>SDSuzFev64</t>
+  </si>
+  <si>
+    <t>SDSuzFev65</t>
+  </si>
+  <si>
+    <t>SDSuzFev66</t>
+  </si>
+  <si>
+    <t>SDSuzFev67</t>
+  </si>
+  <si>
+    <t>SDSuzFev68</t>
+  </si>
+  <si>
+    <t>SDSuzFev69</t>
+  </si>
+  <si>
+    <t>SDSuzFev70</t>
+  </si>
+  <si>
+    <t>SDSuzFev71</t>
+  </si>
+  <si>
+    <t>SDSuzFev72</t>
+  </si>
+  <si>
+    <t>SDSuzFev73</t>
+  </si>
+  <si>
+    <t>SDSuzFev74</t>
+  </si>
+  <si>
+    <t>SDSuzFev75</t>
+  </si>
+  <si>
+    <t>SDSuzFev76</t>
+  </si>
+  <si>
+    <t>SDSuzFev77</t>
+  </si>
+  <si>
+    <t>SDSuzFev78</t>
+  </si>
+  <si>
+    <t>SDSuzApr79</t>
+  </si>
+  <si>
+    <t>SDSuzApr80</t>
+  </si>
+  <si>
+    <t>SDSuzApr81</t>
+  </si>
+  <si>
+    <t>SDSuzApr82</t>
+  </si>
+  <si>
+    <t>SDSuzApr83</t>
+  </si>
+  <si>
+    <t>SDSuzApr84</t>
+  </si>
+  <si>
+    <t>SDSuzApr85</t>
+  </si>
+  <si>
+    <t>SDSuzApr86</t>
+  </si>
+  <si>
+    <t>SDSuzApr87</t>
+  </si>
+  <si>
+    <t>SDSuzApr88</t>
   </si>
 </sst>
 </file>
@@ -1064,7 +1064,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -1075,6 +1075,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1432,7 +1433,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1462,7 +1465,7 @@
       <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
@@ -1489,7 +1492,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="1">
-        <v>44813.489583333336</v>
+        <v>43352.489583333336</v>
       </c>
       <c r="D2">
         <v>-48.995342430000001</v>
@@ -1501,10 +1504,10 @@
         <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="H2" s="1">
-        <v>44813.618055555555</v>
+        <v>43352.618055555555</v>
       </c>
       <c r="I2">
         <v>-48.993802109999997</v>
@@ -1521,13 +1524,13 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="1">
-        <v>44813.489583333336</v>
+        <v>43352.489583333336</v>
       </c>
       <c r="D3">
         <v>-48.995342430000001</v>
@@ -1539,10 +1542,10 @@
         <v>3</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>96</v>
       </c>
       <c r="H3" s="1">
-        <v>44813.621527777781</v>
+        <v>43352.621527777781</v>
       </c>
       <c r="I3">
         <v>-48.993657800000001</v>
@@ -1562,10 +1565,10 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1">
-        <v>44813.489583333336</v>
+        <v>43352.489583333336</v>
       </c>
       <c r="D4">
         <v>-48.995342430000001</v>
@@ -1577,10 +1580,10 @@
         <v>4</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>97</v>
       </c>
       <c r="H4" s="1">
-        <v>44813.618055555555</v>
+        <v>43352.618055555555</v>
       </c>
       <c r="I4">
         <v>-48.993802109999997</v>
@@ -1597,13 +1600,13 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
       <c r="C5" s="1">
-        <v>44813.489583333336</v>
+        <v>43352.489583333336</v>
       </c>
       <c r="D5">
         <v>-48.995342430000001</v>
@@ -1615,10 +1618,10 @@
         <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>98</v>
       </c>
       <c r="H5" s="1">
-        <v>44813.621527777781</v>
+        <v>43352.621527777781</v>
       </c>
       <c r="I5">
         <v>-48.993657800000001</v>
@@ -1638,10 +1641,10 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1">
-        <v>44813.538194444445</v>
+        <v>43352.538194444445</v>
       </c>
       <c r="D6">
         <v>-48.994742870000003</v>
@@ -1653,10 +1656,10 @@
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
+        <v>99</v>
       </c>
       <c r="H6" s="1">
-        <v>44813.618055555555</v>
+        <v>43352.618055555555</v>
       </c>
       <c r="I6">
         <v>-48.993802109999997</v>
@@ -1673,13 +1676,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1">
-        <v>44813.545138888891</v>
+        <v>43352.545138888891</v>
       </c>
       <c r="D7">
         <v>-48.994703199999996</v>
@@ -1691,10 +1694,10 @@
         <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>22</v>
+        <v>100</v>
       </c>
       <c r="H7" s="1">
-        <v>44813.625</v>
+        <v>43352.625</v>
       </c>
       <c r="I7">
         <v>-48.993657800000001</v>
@@ -1711,13 +1714,13 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C8" s="1">
-        <v>44813.628472222219</v>
+        <v>43352.628472222219</v>
       </c>
       <c r="D8">
         <v>-48.993657800000001</v>
@@ -1729,10 +1732,10 @@
         <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
       <c r="H8" s="1">
-        <v>44814.329861111109</v>
+        <v>43353.329861111109</v>
       </c>
       <c r="I8">
         <v>-48.993224810000001</v>
@@ -1749,13 +1752,13 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C9" s="1">
-        <v>44813.631944444445</v>
+        <v>43352.631944444445</v>
       </c>
       <c r="D9">
         <v>-48.993629319999997</v>
@@ -1767,10 +1770,10 @@
         <v>8</v>
       </c>
       <c r="G9" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="H9" s="1">
-        <v>44814.333333333336</v>
+        <v>43353.333333333336</v>
       </c>
       <c r="I9">
         <v>-48.993189200000003</v>
@@ -1787,13 +1790,13 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C10" s="1">
-        <v>44813.697916666664</v>
+        <v>43352.697916666664</v>
       </c>
       <c r="D10">
         <v>-48.99354598</v>
@@ -1805,10 +1808,10 @@
         <v>9</v>
       </c>
       <c r="G10" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
       <c r="H10" s="1">
-        <v>44814.34375</v>
+        <v>43353.34375</v>
       </c>
       <c r="I10">
         <v>-48.993125310000003</v>
@@ -1825,13 +1828,13 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C11" s="1">
-        <v>44813.697916666664</v>
+        <v>43352.697916666664</v>
       </c>
       <c r="D11">
         <v>-48.99354598</v>
@@ -1843,10 +1846,10 @@
         <v>9</v>
       </c>
       <c r="G11" t="s">
-        <v>31</v>
+        <v>104</v>
       </c>
       <c r="H11" s="1">
-        <v>44814.357638888891</v>
+        <v>43353.357638888891</v>
       </c>
       <c r="I11">
         <v>-48.993201130000003</v>
@@ -1863,13 +1866,13 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C12" s="1">
-        <v>44814.583333333336</v>
+        <v>43353.583333333336</v>
       </c>
       <c r="D12">
         <v>-48.993023960000002</v>
@@ -1881,10 +1884,10 @@
         <v>15</v>
       </c>
       <c r="G12" t="s">
-        <v>33</v>
+        <v>105</v>
       </c>
       <c r="H12" s="1">
-        <v>44814.663194444445</v>
+        <v>43353.663194444445</v>
       </c>
       <c r="I12">
         <v>-48.993141659999999</v>
@@ -1901,13 +1904,13 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C13" s="1">
-        <v>44814.677083333336</v>
+        <v>43353.677083333336</v>
       </c>
       <c r="D13">
         <v>-48.993198679999999</v>
@@ -1919,10 +1922,10 @@
         <v>17</v>
       </c>
       <c r="G13" t="s">
-        <v>36</v>
+        <v>106</v>
       </c>
       <c r="H13" s="1">
-        <v>44815.319444444445</v>
+        <v>43354.319444444445</v>
       </c>
       <c r="I13">
         <v>-48.99342867</v>
@@ -1939,13 +1942,13 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C14" s="1">
-        <v>44815.486111111109</v>
+        <v>43354.486111111109</v>
       </c>
       <c r="D14">
         <v>-48.99264367</v>
@@ -1957,10 +1960,10 @@
         <v>21</v>
       </c>
       <c r="G14" t="s">
-        <v>39</v>
+        <v>107</v>
       </c>
       <c r="H14" s="1">
-        <v>44815.569444444445</v>
+        <v>43354.569444444445</v>
       </c>
       <c r="I14">
         <v>-48.992404180000001</v>
@@ -1977,13 +1980,13 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C15" s="1">
-        <v>44815.496527777781</v>
+        <v>43354.496527777781</v>
       </c>
       <c r="D15">
         <v>-48.992633949999998</v>
@@ -1995,10 +1998,10 @@
         <v>22</v>
       </c>
       <c r="G15" t="s">
-        <v>42</v>
+        <v>108</v>
       </c>
       <c r="H15" s="1">
-        <v>44815.59375</v>
+        <v>43354.59375</v>
       </c>
       <c r="I15">
         <v>-48.99268833</v>
@@ -2007,7 +2010,7 @@
         <v>-22.76403766</v>
       </c>
       <c r="K15" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="L15">
         <v>62</v>
@@ -2015,13 +2018,13 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C16" s="1">
-        <v>44815.5625</v>
+        <v>43354.5625</v>
       </c>
       <c r="D16">
         <v>-48.992292229999997</v>
@@ -2033,10 +2036,10 @@
         <v>23</v>
       </c>
       <c r="G16" t="s">
-        <v>45</v>
+        <v>109</v>
       </c>
       <c r="H16" s="1">
-        <v>44815.59375</v>
+        <v>43354.59375</v>
       </c>
       <c r="I16">
         <v>-48.99268833</v>
@@ -2053,13 +2056,13 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C17" s="1">
-        <v>44815.5625</v>
+        <v>43354.5625</v>
       </c>
       <c r="D17">
         <v>-48.992292229999997</v>
@@ -2071,10 +2074,10 @@
         <v>23</v>
       </c>
       <c r="G17" t="s">
-        <v>47</v>
+        <v>110</v>
       </c>
       <c r="H17" s="1">
-        <v>44815.607638888891</v>
+        <v>43354.607638888891</v>
       </c>
       <c r="I17">
         <v>-48.99278588</v>
@@ -2091,13 +2094,13 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C18" s="1">
-        <v>44815.576388888891</v>
+        <v>43354.576388888891</v>
       </c>
       <c r="D18">
         <v>-48.992552459999999</v>
@@ -2109,10 +2112,10 @@
         <v>24</v>
       </c>
       <c r="G18" t="s">
-        <v>49</v>
+        <v>111</v>
       </c>
       <c r="H18" s="1">
-        <v>44815.59375</v>
+        <v>43354.59375</v>
       </c>
       <c r="I18">
         <v>-48.99268833</v>
@@ -2129,13 +2132,13 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C19" s="1">
-        <v>44815.576388888891</v>
+        <v>43354.576388888891</v>
       </c>
       <c r="D19">
         <v>-48.99261327</v>
@@ -2147,10 +2150,10 @@
         <v>25</v>
       </c>
       <c r="G19" t="s">
-        <v>51</v>
+        <v>112</v>
       </c>
       <c r="H19" s="1">
-        <v>44815.680555555555</v>
+        <v>43354.680555555555</v>
       </c>
       <c r="I19">
         <v>-48.993309009999997</v>
@@ -2167,13 +2170,13 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C20" s="1">
-        <v>44816.340277777781</v>
+        <v>43355.340277777781</v>
       </c>
       <c r="D20">
         <v>-48.993463769999998</v>
@@ -2185,10 +2188,10 @@
         <v>29</v>
       </c>
       <c r="G20" t="s">
-        <v>53</v>
+        <v>113</v>
       </c>
       <c r="H20" s="1">
-        <v>44816.420138888891</v>
+        <v>43355.420138888891</v>
       </c>
       <c r="I20">
         <v>-48.993868999999997</v>
@@ -2205,13 +2208,13 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C21" s="1">
-        <v>44816.340277777781</v>
+        <v>43355.340277777781</v>
       </c>
       <c r="D21">
         <v>-48.993463769999998</v>
@@ -2223,10 +2226,10 @@
         <v>29</v>
       </c>
       <c r="G21" t="s">
-        <v>55</v>
+        <v>114</v>
       </c>
       <c r="H21" s="1">
-        <v>44816.430555555555</v>
+        <v>43355.430555555555</v>
       </c>
       <c r="I21">
         <v>-48.993927810000002</v>
@@ -2243,13 +2246,13 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="C22" s="1">
-        <v>44816.46875</v>
+        <v>43355.46875</v>
       </c>
       <c r="D22">
         <v>-48.994121270000001</v>
@@ -2261,10 +2264,10 @@
         <v>30</v>
       </c>
       <c r="G22" t="s">
-        <v>58</v>
+        <v>115</v>
       </c>
       <c r="H22" s="1">
-        <v>44816.579861111109</v>
+        <v>43355.579861111109</v>
       </c>
       <c r="I22">
         <v>-48.993888750000004</v>
@@ -2281,13 +2284,13 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="C23" s="1">
-        <v>44816.46875</v>
+        <v>43355.46875</v>
       </c>
       <c r="D23">
         <v>-48.994121270000001</v>
@@ -2299,10 +2302,10 @@
         <v>30</v>
       </c>
       <c r="G23" t="s">
-        <v>60</v>
+        <v>116</v>
       </c>
       <c r="H23" s="1">
-        <v>44816.586805555555</v>
+        <v>43355.586805555555</v>
       </c>
       <c r="I23">
         <v>-48.993740500000001</v>
@@ -2319,13 +2322,13 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C24" s="1">
-        <v>44816.479166666664</v>
+        <v>43355.479166666664</v>
       </c>
       <c r="D24">
         <v>-48.994082329999998</v>
@@ -2337,10 +2340,10 @@
         <v>31</v>
       </c>
       <c r="G24" t="s">
-        <v>61</v>
+        <v>117</v>
       </c>
       <c r="H24" s="1">
-        <v>44816.579861111109</v>
+        <v>43355.579861111109</v>
       </c>
       <c r="I24">
         <v>-48.993888750000004</v>
@@ -2349,7 +2352,7 @@
         <v>-22.7630537</v>
       </c>
       <c r="K24" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="L24">
         <v>120</v>
@@ -2357,13 +2360,13 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C25" s="1">
-        <v>44816.479166666664</v>
+        <v>43355.479166666664</v>
       </c>
       <c r="D25">
         <v>-48.994082329999998</v>
@@ -2375,10 +2378,10 @@
         <v>31</v>
       </c>
       <c r="G25" t="s">
-        <v>62</v>
+        <v>118</v>
       </c>
       <c r="H25" s="1">
-        <v>44816.586805555555</v>
+        <v>43355.586805555555</v>
       </c>
       <c r="I25">
         <v>-48.993740500000001</v>
@@ -2387,7 +2390,7 @@
         <v>-22.763368140000001</v>
       </c>
       <c r="K25" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="L25">
         <v>154</v>
@@ -2395,13 +2398,13 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C26" s="1">
-        <v>44902.309027777781</v>
+        <v>43441.309027777781</v>
       </c>
       <c r="D26">
         <v>-48.993737889999998</v>
@@ -2413,10 +2416,10 @@
         <v>38</v>
       </c>
       <c r="G26" t="s">
-        <v>64</v>
+        <v>119</v>
       </c>
       <c r="H26" s="1">
-        <v>44902.399305555555</v>
+        <v>43441.399305555555</v>
       </c>
       <c r="I26">
         <v>-48.994317559999999</v>
@@ -2433,13 +2436,13 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="B27" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C27" s="1">
-        <v>44902.309027777781</v>
+        <v>43441.309027777781</v>
       </c>
       <c r="D27">
         <v>-48.993737889999998</v>
@@ -2451,10 +2454,10 @@
         <v>38</v>
       </c>
       <c r="G27" t="s">
-        <v>66</v>
+        <v>120</v>
       </c>
       <c r="H27" s="1">
-        <v>44902.427083333336</v>
+        <v>43441.427083333336</v>
       </c>
       <c r="I27">
         <v>-48.994461690000001</v>
@@ -2471,13 +2474,13 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="B28" t="s">
         <v>13</v>
       </c>
       <c r="C28" s="1">
-        <v>44902.399305555555</v>
+        <v>43441.399305555555</v>
       </c>
       <c r="D28">
         <v>-48.994317559999999</v>
@@ -2489,10 +2492,10 @@
         <v>40</v>
       </c>
       <c r="G28" t="s">
-        <v>68</v>
+        <v>121</v>
       </c>
       <c r="H28" s="1">
-        <v>44902.482638888891</v>
+        <v>43441.482638888891</v>
       </c>
       <c r="I28">
         <v>-48.995004940000001</v>
@@ -2509,13 +2512,13 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="B29" t="s">
         <v>13</v>
       </c>
       <c r="C29" s="1">
-        <v>44902.399305555555</v>
+        <v>43441.399305555555</v>
       </c>
       <c r="D29">
         <v>-48.994317559999999</v>
@@ -2527,10 +2530,10 @@
         <v>40</v>
       </c>
       <c r="G29" t="s">
-        <v>70</v>
+        <v>122</v>
       </c>
       <c r="H29" s="1">
-        <v>44902.510416666664</v>
+        <v>43441.510416666664</v>
       </c>
       <c r="I29">
         <v>-48.995207010000001</v>
@@ -2547,13 +2550,13 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="B30" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C30" s="1">
-        <v>44902.409722222219</v>
+        <v>43441.409722222219</v>
       </c>
       <c r="D30">
         <v>-48.994269979999999</v>
@@ -2565,10 +2568,10 @@
         <v>41</v>
       </c>
       <c r="G30" t="s">
-        <v>71</v>
+        <v>123</v>
       </c>
       <c r="H30" s="1">
-        <v>44902.510416666664</v>
+        <v>43441.510416666664</v>
       </c>
       <c r="I30">
         <v>-48.995207010000001</v>
@@ -2585,13 +2588,13 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="B31" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C31" s="1">
-        <v>44902.510416666664</v>
+        <v>43441.510416666664</v>
       </c>
       <c r="D31">
         <v>-48.995207010000001</v>
@@ -2603,10 +2606,10 @@
         <v>44</v>
       </c>
       <c r="G31" t="s">
-        <v>73</v>
+        <v>124</v>
       </c>
       <c r="H31" s="1">
-        <v>44902.572916666664</v>
+        <v>43441.572916666664</v>
       </c>
       <c r="I31">
         <v>-48.99460165</v>
@@ -2623,13 +2626,13 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C32" s="1">
-        <v>44902.510416666664</v>
+        <v>43441.510416666664</v>
       </c>
       <c r="D32">
         <v>-48.995207010000001</v>
@@ -2641,10 +2644,10 @@
         <v>44</v>
       </c>
       <c r="G32" t="s">
-        <v>75</v>
+        <v>125</v>
       </c>
       <c r="H32" s="1">
-        <v>44902.583333333336</v>
+        <v>43441.583333333336</v>
       </c>
       <c r="I32">
         <v>-48.994500739999999</v>
@@ -2661,13 +2664,13 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
       <c r="B33" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C33" s="1">
-        <v>44902.510416666664</v>
+        <v>43441.510416666664</v>
       </c>
       <c r="D33">
         <v>-48.995207010000001</v>
@@ -2679,10 +2682,10 @@
         <v>44</v>
       </c>
       <c r="G33" t="s">
-        <v>77</v>
+        <v>126</v>
       </c>
       <c r="H33" s="1">
-        <v>44902.600694444445</v>
+        <v>43441.600694444445</v>
       </c>
       <c r="I33">
         <v>-48.994441049999999</v>
@@ -2699,13 +2702,13 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="B34" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="C34" s="1">
-        <v>44902.520833333336</v>
+        <v>43441.520833333336</v>
       </c>
       <c r="D34">
         <v>-48.995207010000001</v>
@@ -2717,10 +2720,10 @@
         <v>45</v>
       </c>
       <c r="G34" t="s">
-        <v>79</v>
+        <v>127</v>
       </c>
       <c r="H34" s="1">
-        <v>44902.572916666664</v>
+        <v>43441.572916666664</v>
       </c>
       <c r="I34">
         <v>-48.99460165</v>
@@ -2737,13 +2740,13 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="B35" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="C35" s="1">
-        <v>44902.520833333336</v>
+        <v>43441.520833333336</v>
       </c>
       <c r="D35">
         <v>-48.995207010000001</v>
@@ -2755,10 +2758,10 @@
         <v>45</v>
       </c>
       <c r="G35" t="s">
-        <v>80</v>
+        <v>128</v>
       </c>
       <c r="H35" s="1">
-        <v>44902.583333333336</v>
+        <v>43441.583333333336</v>
       </c>
       <c r="I35">
         <v>-48.994500739999999</v>
@@ -2775,13 +2778,13 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
       <c r="B36" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="C36" s="1">
-        <v>44902.520833333336</v>
+        <v>43441.520833333336</v>
       </c>
       <c r="D36">
         <v>-48.995207010000001</v>
@@ -2793,10 +2796,10 @@
         <v>45</v>
       </c>
       <c r="G36" t="s">
-        <v>81</v>
+        <v>129</v>
       </c>
       <c r="H36" s="1">
-        <v>44902.600694444445</v>
+        <v>43441.600694444445</v>
       </c>
       <c r="I36">
         <v>-48.994441049999999</v>
@@ -2813,13 +2816,13 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>82</v>
+        <v>47</v>
       </c>
       <c r="B37" t="s">
         <v>13</v>
       </c>
       <c r="C37" s="1">
-        <v>44902.635416666664</v>
+        <v>43441.635416666664</v>
       </c>
       <c r="D37">
         <v>-48.994267729999997</v>
@@ -2831,10 +2834,10 @@
         <v>47</v>
       </c>
       <c r="G37" t="s">
-        <v>83</v>
+        <v>130</v>
       </c>
       <c r="H37" s="1">
-        <v>44902.725694444445</v>
+        <v>43441.725694444445</v>
       </c>
       <c r="I37">
         <v>-48.993462010000002</v>
@@ -2851,13 +2854,13 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="B38" t="s">
         <v>13</v>
       </c>
       <c r="C38" s="1">
-        <v>44902.635416666664</v>
+        <v>43441.635416666664</v>
       </c>
       <c r="D38">
         <v>-48.994267729999997</v>
@@ -2869,10 +2872,10 @@
         <v>47</v>
       </c>
       <c r="G38" t="s">
-        <v>85</v>
+        <v>131</v>
       </c>
       <c r="H38" s="1">
-        <v>44902.725694444445</v>
+        <v>43441.725694444445</v>
       </c>
       <c r="I38">
         <v>-48.993462010000002</v>
@@ -2889,13 +2892,13 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="B39" t="s">
         <v>13</v>
       </c>
       <c r="C39" s="1">
-        <v>44902.711805555555</v>
+        <v>43441.711805555555</v>
       </c>
       <c r="D39">
         <v>-48.993473360000003</v>
@@ -2907,10 +2910,10 @@
         <v>49</v>
       </c>
       <c r="G39" t="s">
-        <v>87</v>
+        <v>132</v>
       </c>
       <c r="H39" s="1">
-        <v>44903.315972222219</v>
+        <v>43442.315972222219</v>
       </c>
       <c r="I39">
         <v>-48.993229880000001</v>
@@ -2927,13 +2930,13 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="B40" t="s">
         <v>13</v>
       </c>
       <c r="C40" s="1">
-        <v>44902.711805555555</v>
+        <v>43441.711805555555</v>
       </c>
       <c r="D40">
         <v>-48.993473360000003</v>
@@ -2945,10 +2948,10 @@
         <v>49</v>
       </c>
       <c r="G40" t="s">
-        <v>89</v>
+        <v>133</v>
       </c>
       <c r="H40" s="1">
-        <v>44903.347222222219</v>
+        <v>43442.347222222219</v>
       </c>
       <c r="I40">
         <v>-48.99376032</v>
@@ -2965,13 +2968,13 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>90</v>
+        <v>51</v>
       </c>
       <c r="B41" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C41" s="1">
-        <v>44903.385416666664</v>
+        <v>43442.385416666664</v>
       </c>
       <c r="D41">
         <v>-48.99397982</v>
@@ -2983,10 +2986,10 @@
         <v>50</v>
       </c>
       <c r="G41" t="s">
-        <v>91</v>
+        <v>134</v>
       </c>
       <c r="H41" s="1">
-        <v>44903.4375</v>
+        <v>43442.4375</v>
       </c>
       <c r="I41">
         <v>-48.993346219999999</v>
@@ -3003,13 +3006,13 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>92</v>
+        <v>52</v>
       </c>
       <c r="B42" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C42" s="1">
-        <v>44903.385416666664</v>
+        <v>43442.385416666664</v>
       </c>
       <c r="D42">
         <v>-48.99397982</v>
@@ -3021,10 +3024,10 @@
         <v>50</v>
       </c>
       <c r="G42" t="s">
-        <v>93</v>
+        <v>135</v>
       </c>
       <c r="H42" s="1">
-        <v>44903.451388888891</v>
+        <v>43442.451388888891</v>
       </c>
       <c r="I42">
         <v>-48.99379407</v>
@@ -3041,13 +3044,13 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>90</v>
+        <v>51</v>
       </c>
       <c r="B43" t="s">
         <v>13</v>
       </c>
       <c r="C43" s="1">
-        <v>44903.413194444445</v>
+        <v>43442.413194444445</v>
       </c>
       <c r="D43">
         <v>-48.993354500000002</v>
@@ -3059,10 +3062,10 @@
         <v>51</v>
       </c>
       <c r="G43" t="s">
-        <v>94</v>
+        <v>136</v>
       </c>
       <c r="H43" s="1">
-        <v>44903.4375</v>
+        <v>43442.4375</v>
       </c>
       <c r="I43">
         <v>-48.993346219999999</v>
@@ -3079,13 +3082,13 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>95</v>
+        <v>53</v>
       </c>
       <c r="B44" t="s">
-        <v>96</v>
+        <v>54</v>
       </c>
       <c r="C44" s="1">
-        <v>44903.649305555555</v>
+        <v>43442.649305555555</v>
       </c>
       <c r="D44">
         <v>-48.993572129999997</v>
@@ -3097,10 +3100,10 @@
         <v>54</v>
       </c>
       <c r="G44" t="s">
-        <v>97</v>
+        <v>137</v>
       </c>
       <c r="H44" s="1">
-        <v>44904.350694444445</v>
+        <v>43443.350694444445</v>
       </c>
       <c r="I44">
         <v>-48.993904710000002</v>
@@ -3117,13 +3120,13 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="B45" t="s">
-        <v>96</v>
+        <v>54</v>
       </c>
       <c r="C45" s="1">
-        <v>44903.666666666664</v>
+        <v>43442.666666666664</v>
       </c>
       <c r="D45">
         <v>-48.993351590000003</v>
@@ -3135,10 +3138,10 @@
         <v>55</v>
       </c>
       <c r="G45" t="s">
-        <v>99</v>
+        <v>138</v>
       </c>
       <c r="H45" s="1">
-        <v>44904.350694444445</v>
+        <v>43443.350694444445</v>
       </c>
       <c r="I45">
         <v>-48.993904710000002</v>
@@ -3155,13 +3158,13 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>100</v>
+        <v>56</v>
       </c>
       <c r="B46" t="s">
         <v>13</v>
       </c>
       <c r="C46" s="1">
-        <v>44904.548611111109</v>
+        <v>43443.548611111109</v>
       </c>
       <c r="D46">
         <v>-48.995160329999997</v>
@@ -3173,10 +3176,10 @@
         <v>58</v>
       </c>
       <c r="G46" t="s">
-        <v>101</v>
+        <v>139</v>
       </c>
       <c r="H46" s="1">
-        <v>44904.614583333336</v>
+        <v>43443.614583333336</v>
       </c>
       <c r="I46">
         <v>-48.993649730000001</v>
@@ -3193,13 +3196,13 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>102</v>
+        <v>57</v>
       </c>
       <c r="B47" t="s">
         <v>13</v>
       </c>
       <c r="C47" s="1">
-        <v>44904.548611111109</v>
+        <v>43443.548611111109</v>
       </c>
       <c r="D47">
         <v>-48.995160329999997</v>
@@ -3211,10 +3214,10 @@
         <v>58</v>
       </c>
       <c r="G47" t="s">
-        <v>103</v>
+        <v>140</v>
       </c>
       <c r="H47" s="1">
-        <v>44904.642361111109</v>
+        <v>43443.642361111109</v>
       </c>
       <c r="I47">
         <v>-48.99320908</v>
@@ -3231,13 +3234,13 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>100</v>
+        <v>56</v>
       </c>
       <c r="B48" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="C48" s="1">
-        <v>44904.548611111109</v>
+        <v>43443.548611111109</v>
       </c>
       <c r="D48">
         <v>-48.995160329999997</v>
@@ -3249,10 +3252,10 @@
         <v>59</v>
       </c>
       <c r="G48" t="s">
-        <v>104</v>
+        <v>141</v>
       </c>
       <c r="H48" s="1">
-        <v>44904.614583333336</v>
+        <v>43443.614583333336</v>
       </c>
       <c r="I48">
         <v>-48.993649730000001</v>
@@ -3269,13 +3272,13 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>102</v>
+        <v>57</v>
       </c>
       <c r="B49" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="C49" s="1">
-        <v>44904.548611111109</v>
+        <v>43443.548611111109</v>
       </c>
       <c r="D49">
         <v>-48.995160329999997</v>
@@ -3287,10 +3290,10 @@
         <v>59</v>
       </c>
       <c r="G49" t="s">
-        <v>105</v>
+        <v>142</v>
       </c>
       <c r="H49" s="1">
-        <v>44904.642361111109</v>
+        <v>43443.642361111109</v>
       </c>
       <c r="I49">
         <v>-48.99320908</v>
@@ -3307,13 +3310,13 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>106</v>
+        <v>58</v>
       </c>
       <c r="B50" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C50" s="1">
-        <v>44905.444444444445</v>
+        <v>43444.444444444445</v>
       </c>
       <c r="D50">
         <v>-48.99409824</v>
@@ -3325,10 +3328,10 @@
         <v>67</v>
       </c>
       <c r="G50" t="s">
-        <v>107</v>
+        <v>143</v>
       </c>
       <c r="H50" s="1">
-        <v>44905.503472222219</v>
+        <v>43444.503472222219</v>
       </c>
       <c r="I50">
         <v>-48.994872350000001</v>
@@ -3345,13 +3348,13 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>108</v>
+        <v>59</v>
       </c>
       <c r="B51" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C51" s="1">
-        <v>44905.444444444445</v>
+        <v>43444.444444444445</v>
       </c>
       <c r="D51">
         <v>-48.99409824</v>
@@ -3363,10 +3366,10 @@
         <v>67</v>
       </c>
       <c r="G51" t="s">
-        <v>109</v>
+        <v>144</v>
       </c>
       <c r="H51" s="1">
-        <v>44905.538194444445</v>
+        <v>43444.538194444445</v>
       </c>
       <c r="I51">
         <v>-48.994877449999997</v>
@@ -3383,13 +3386,13 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="B52" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="C52" s="1">
-        <v>44906.524305555555</v>
+        <v>43445.524305555555</v>
       </c>
       <c r="D52">
         <v>-48.996441760000003</v>
@@ -3401,10 +3404,10 @@
         <v>74</v>
       </c>
       <c r="G52" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="H52" s="1">
-        <v>44906.663194444445</v>
+        <v>43445.663194444445</v>
       </c>
       <c r="I52">
         <v>-48.99419743</v>
@@ -3421,13 +3424,13 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="B53" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C53" s="1">
-        <v>44906.555555555555</v>
+        <v>43445.555555555555</v>
       </c>
       <c r="D53">
         <v>-48.996403870000002</v>
@@ -3439,10 +3442,10 @@
         <v>75</v>
       </c>
       <c r="G53" t="s">
-        <v>112</v>
+        <v>146</v>
       </c>
       <c r="H53" s="1">
-        <v>44906.663194444445</v>
+        <v>43445.663194444445</v>
       </c>
       <c r="I53">
         <v>-48.99419743</v>
@@ -3459,13 +3462,13 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>113</v>
+        <v>61</v>
       </c>
       <c r="B54" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C54" s="1">
-        <v>44907.447916666664</v>
+        <v>43446.447916666664</v>
       </c>
       <c r="D54">
         <v>-48.995943330000003</v>
@@ -3477,10 +3480,10 @@
         <v>77</v>
       </c>
       <c r="G54" t="s">
-        <v>114</v>
+        <v>147</v>
       </c>
       <c r="H54" s="1">
-        <v>44907.46875</v>
+        <v>43446.46875</v>
       </c>
       <c r="I54">
         <v>-48.996503789999998</v>
@@ -3497,13 +3500,13 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>113</v>
+        <v>61</v>
       </c>
       <c r="B55" t="s">
         <v>13</v>
       </c>
       <c r="C55" s="1">
-        <v>44907.447916666664</v>
+        <v>43446.447916666664</v>
       </c>
       <c r="D55">
         <v>-48.995943330000003</v>
@@ -3515,10 +3518,10 @@
         <v>78</v>
       </c>
       <c r="G55" t="s">
-        <v>115</v>
+        <v>148</v>
       </c>
       <c r="H55" s="1">
-        <v>44907.46875</v>
+        <v>43446.46875</v>
       </c>
       <c r="I55">
         <v>-48.996503789999998</v>
@@ -3535,13 +3538,13 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>116</v>
+        <v>62</v>
       </c>
       <c r="B56" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C56" s="1">
-        <v>44907.451388888891</v>
+        <v>43446.451388888891</v>
       </c>
       <c r="D56">
         <v>-48.995943330000003</v>
@@ -3553,10 +3556,10 @@
         <v>77</v>
       </c>
       <c r="G56" t="s">
-        <v>117</v>
+        <v>149</v>
       </c>
       <c r="H56" s="1">
-        <v>44907.482638888891</v>
+        <v>43446.482638888891</v>
       </c>
       <c r="I56">
         <v>-48.99659406</v>
@@ -3573,13 +3576,13 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>116</v>
+        <v>62</v>
       </c>
       <c r="B57" t="s">
         <v>13</v>
       </c>
       <c r="C57" s="1">
-        <v>44907.451388888891</v>
+        <v>43446.451388888891</v>
       </c>
       <c r="D57">
         <v>-48.995943330000003</v>
@@ -3591,10 +3594,10 @@
         <v>78</v>
       </c>
       <c r="G57" t="s">
-        <v>118</v>
+        <v>150</v>
       </c>
       <c r="H57" s="1">
-        <v>44907.482638888891</v>
+        <v>43446.482638888891</v>
       </c>
       <c r="I57">
         <v>-48.99659406</v>
@@ -3611,13 +3614,13 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>119</v>
+        <v>63</v>
       </c>
       <c r="B58" t="s">
-        <v>120</v>
+        <v>64</v>
       </c>
       <c r="C58" s="1">
-        <v>44976.357638888891</v>
+        <v>43515.357638888891</v>
       </c>
       <c r="D58">
         <v>-48.995732449999998</v>
@@ -3629,10 +3632,10 @@
         <v>81</v>
       </c>
       <c r="G58" t="s">
-        <v>121</v>
+        <v>151</v>
       </c>
       <c r="H58" s="1">
-        <v>44976.4375</v>
+        <v>43515.4375</v>
       </c>
       <c r="I58">
         <v>-48.997744060000002</v>
@@ -3649,13 +3652,13 @@
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>122</v>
+        <v>65</v>
       </c>
       <c r="B59" t="s">
-        <v>120</v>
+        <v>64</v>
       </c>
       <c r="C59" s="1">
-        <v>44976.357638888891</v>
+        <v>43515.357638888891</v>
       </c>
       <c r="D59">
         <v>-48.995732449999998</v>
@@ -3667,10 +3670,10 @@
         <v>81</v>
       </c>
       <c r="G59" t="s">
-        <v>123</v>
+        <v>152</v>
       </c>
       <c r="H59" s="1">
-        <v>44976.444444444445</v>
+        <v>43515.444444444445</v>
       </c>
       <c r="I59">
         <v>-48.997904830000003</v>
@@ -3687,13 +3690,13 @@
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>119</v>
+        <v>63</v>
       </c>
       <c r="B60" t="s">
-        <v>124</v>
+        <v>66</v>
       </c>
       <c r="C60" s="1">
-        <v>44976.364583333336</v>
+        <v>43515.364583333336</v>
       </c>
       <c r="D60">
         <v>-48.995850730000001</v>
@@ -3705,10 +3708,10 @@
         <v>82</v>
       </c>
       <c r="G60" t="s">
-        <v>125</v>
+        <v>153</v>
       </c>
       <c r="H60" s="1">
-        <v>44976.4375</v>
+        <v>43515.4375</v>
       </c>
       <c r="I60">
         <v>-48.997744060000002</v>
@@ -3725,13 +3728,13 @@
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>122</v>
+        <v>65</v>
       </c>
       <c r="B61" t="s">
-        <v>124</v>
+        <v>66</v>
       </c>
       <c r="C61" s="1">
-        <v>44976.364583333336</v>
+        <v>43515.364583333336</v>
       </c>
       <c r="D61">
         <v>-48.995850730000001</v>
@@ -3743,10 +3746,10 @@
         <v>82</v>
       </c>
       <c r="G61" t="s">
-        <v>126</v>
+        <v>154</v>
       </c>
       <c r="H61" s="1">
-        <v>44976.444444444445</v>
+        <v>43515.444444444445</v>
       </c>
       <c r="I61">
         <v>-48.997904830000003</v>
@@ -3763,13 +3766,13 @@
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>127</v>
+        <v>67</v>
       </c>
       <c r="B62" t="s">
-        <v>124</v>
+        <v>66</v>
       </c>
       <c r="C62" s="1">
-        <v>44976.454861111109</v>
+        <v>43515.454861111109</v>
       </c>
       <c r="D62">
         <v>-48.997605819999997</v>
@@ -3781,10 +3784,10 @@
         <v>83</v>
       </c>
       <c r="G62" t="s">
-        <v>128</v>
+        <v>155</v>
       </c>
       <c r="H62" s="1">
-        <v>44976.552083333336</v>
+        <v>43515.552083333336</v>
       </c>
       <c r="I62">
         <v>-48.998115480000003</v>
@@ -3801,13 +3804,13 @@
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>129</v>
+        <v>68</v>
       </c>
       <c r="B63" t="s">
-        <v>120</v>
+        <v>64</v>
       </c>
       <c r="C63" s="1">
-        <v>44976.472222222219</v>
+        <v>43515.472222222219</v>
       </c>
       <c r="D63">
         <v>-48.997469240000001</v>
@@ -3819,10 +3822,10 @@
         <v>84</v>
       </c>
       <c r="G63" t="s">
-        <v>130</v>
+        <v>156</v>
       </c>
       <c r="H63" s="1">
-        <v>44976.579861111109</v>
+        <v>43515.579861111109</v>
       </c>
       <c r="I63">
         <v>-48.997983300000001</v>
@@ -3839,13 +3842,13 @@
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>131</v>
+        <v>69</v>
       </c>
       <c r="B64" t="s">
-        <v>124</v>
+        <v>66</v>
       </c>
       <c r="C64" s="1">
-        <v>44976.552083333336</v>
+        <v>43515.552083333336</v>
       </c>
       <c r="D64">
         <v>-48.998115480000003</v>
@@ -3857,10 +3860,10 @@
         <v>86</v>
       </c>
       <c r="G64" t="s">
-        <v>132</v>
+        <v>157</v>
       </c>
       <c r="H64" s="1">
-        <v>44976.631944444445</v>
+        <v>43515.631944444445</v>
       </c>
       <c r="I64">
         <v>-48.997880790000004</v>
@@ -3877,13 +3880,13 @@
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>133</v>
+        <v>70</v>
       </c>
       <c r="B65" t="s">
-        <v>134</v>
+        <v>71</v>
       </c>
       <c r="C65" s="1">
-        <v>44976.635416666664</v>
+        <v>43515.635416666664</v>
       </c>
       <c r="D65">
         <v>-48.997904159999997</v>
@@ -3895,10 +3898,10 @@
         <v>87</v>
       </c>
       <c r="G65" t="s">
-        <v>135</v>
+        <v>158</v>
       </c>
       <c r="H65" s="1">
-        <v>44977.347222222219</v>
+        <v>43516.347222222219</v>
       </c>
       <c r="I65">
         <v>-48.999416570000001</v>
@@ -3915,13 +3918,13 @@
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>136</v>
+        <v>72</v>
       </c>
       <c r="B66" t="s">
-        <v>134</v>
+        <v>71</v>
       </c>
       <c r="C66" s="1">
-        <v>44976.635416666664</v>
+        <v>43515.635416666664</v>
       </c>
       <c r="D66">
         <v>-48.997904159999997</v>
@@ -3933,10 +3936,10 @@
         <v>87</v>
       </c>
       <c r="G66" t="s">
-        <v>137</v>
+        <v>159</v>
       </c>
       <c r="H66" s="1">
-        <v>44977.350694444445</v>
+        <v>43516.350694444445</v>
       </c>
       <c r="I66">
         <v>-48.999504629999997</v>
@@ -3953,13 +3956,13 @@
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>133</v>
+        <v>70</v>
       </c>
       <c r="B67" t="s">
-        <v>138</v>
+        <v>73</v>
       </c>
       <c r="C67" s="1">
-        <v>44976.649305555555</v>
+        <v>43515.649305555555</v>
       </c>
       <c r="D67">
         <v>-48.998105840000001</v>
@@ -3971,10 +3974,10 @@
         <v>88</v>
       </c>
       <c r="G67" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="H67" s="1">
-        <v>44977.347222222219</v>
+        <v>43516.347222222219</v>
       </c>
       <c r="I67">
         <v>-48.999416570000001</v>
@@ -3991,13 +3994,13 @@
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>136</v>
+        <v>72</v>
       </c>
       <c r="B68" t="s">
-        <v>138</v>
+        <v>73</v>
       </c>
       <c r="C68" s="1">
-        <v>44976.649305555555</v>
+        <v>43515.649305555555</v>
       </c>
       <c r="D68">
         <v>-48.998105840000001</v>
@@ -4009,10 +4012,10 @@
         <v>88</v>
       </c>
       <c r="G68" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
       <c r="H68" s="1">
-        <v>44977.350694444445</v>
+        <v>43516.350694444445</v>
       </c>
       <c r="I68">
         <v>-48.999504629999997</v>
@@ -4029,13 +4032,13 @@
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>141</v>
+        <v>74</v>
       </c>
       <c r="B69" t="s">
-        <v>120</v>
+        <v>64</v>
       </c>
       <c r="C69" s="1">
-        <v>44977.350694444445</v>
+        <v>43516.350694444445</v>
       </c>
       <c r="D69">
         <v>-48.999504629999997</v>
@@ -4047,10 +4050,10 @@
         <v>89</v>
       </c>
       <c r="G69" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="H69" s="1">
-        <v>44977.4375</v>
+        <v>43516.4375</v>
       </c>
       <c r="I69">
         <v>-49.00003976</v>
@@ -4067,13 +4070,13 @@
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>141</v>
+        <v>74</v>
       </c>
       <c r="B70" t="s">
-        <v>124</v>
+        <v>66</v>
       </c>
       <c r="C70" s="1">
-        <v>44977.361111111109</v>
+        <v>43516.361111111109</v>
       </c>
       <c r="D70">
         <v>-48.999521590000001</v>
@@ -4085,10 +4088,10 @@
         <v>90</v>
       </c>
       <c r="G70" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
       <c r="H70" s="1">
-        <v>44977.4375</v>
+        <v>43516.4375</v>
       </c>
       <c r="I70">
         <v>-49.00003976</v>
@@ -4105,13 +4108,13 @@
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>144</v>
+        <v>75</v>
       </c>
       <c r="B71" t="s">
-        <v>145</v>
+        <v>76</v>
       </c>
       <c r="C71" s="1">
-        <v>44977.444444444445</v>
+        <v>43516.444444444445</v>
       </c>
       <c r="D71">
         <v>-49.000087669999999</v>
@@ -4123,10 +4126,10 @@
         <v>93</v>
       </c>
       <c r="G71" t="s">
-        <v>146</v>
+        <v>164</v>
       </c>
       <c r="H71" s="1">
-        <v>44977.472222222219</v>
+        <v>43516.472222222219</v>
       </c>
       <c r="I71">
         <v>-48.999708660000003</v>
@@ -4135,7 +4138,7 @@
         <v>-22.764785310000001</v>
       </c>
       <c r="K71" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="L71">
         <v>96</v>
@@ -4143,13 +4146,13 @@
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>147</v>
+        <v>77</v>
       </c>
       <c r="B72" t="s">
-        <v>138</v>
+        <v>73</v>
       </c>
       <c r="C72" s="1">
-        <v>44977.590277777781</v>
+        <v>43516.590277777781</v>
       </c>
       <c r="D72">
         <v>-48.999215640000003</v>
@@ -4161,10 +4164,10 @@
         <v>95</v>
       </c>
       <c r="G72" t="s">
-        <v>148</v>
+        <v>165</v>
       </c>
       <c r="H72" s="1">
-        <v>44977.708333333336</v>
+        <v>43516.708333333336</v>
       </c>
       <c r="I72">
         <v>-48.996641400000001</v>
@@ -4181,13 +4184,13 @@
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>147</v>
+        <v>77</v>
       </c>
       <c r="B73" t="s">
-        <v>120</v>
+        <v>64</v>
       </c>
       <c r="C73" s="1">
-        <v>44977.618055555555</v>
+        <v>43516.618055555555</v>
       </c>
       <c r="D73">
         <v>-48.998619840000003</v>
@@ -4199,10 +4202,10 @@
         <v>96</v>
       </c>
       <c r="G73" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
       <c r="H73" s="1">
-        <v>44977.708333333336</v>
+        <v>43516.708333333336</v>
       </c>
       <c r="I73">
         <v>-48.996641400000001</v>
@@ -4219,13 +4222,13 @@
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>150</v>
+        <v>78</v>
       </c>
       <c r="B74" t="s">
         <v>13</v>
       </c>
       <c r="C74" s="1">
-        <v>44978.381944444445</v>
+        <v>43517.381944444445</v>
       </c>
       <c r="D74">
         <v>-48.996229530000001</v>
@@ -4237,10 +4240,10 @@
         <v>99</v>
       </c>
       <c r="G74" t="s">
-        <v>151</v>
+        <v>167</v>
       </c>
       <c r="H74" s="1">
-        <v>44978.611111111109</v>
+        <v>43517.611111111109</v>
       </c>
       <c r="I74">
         <v>-48.993713120000002</v>
@@ -4257,13 +4260,13 @@
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>152</v>
+        <v>79</v>
       </c>
       <c r="B75" t="s">
-        <v>153</v>
+        <v>80</v>
       </c>
       <c r="C75" s="1">
-        <v>44978.489583333336</v>
+        <v>43517.489583333336</v>
       </c>
       <c r="D75">
         <v>-48.995236630000001</v>
@@ -4275,10 +4278,10 @@
         <v>100</v>
       </c>
       <c r="G75" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="H75" s="1">
-        <v>44978.621527777781</v>
+        <v>43517.621527777781</v>
       </c>
       <c r="I75">
         <v>-48.993211109999997</v>
@@ -4295,13 +4298,13 @@
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>152</v>
+        <v>79</v>
       </c>
       <c r="B76" t="s">
-        <v>120</v>
+        <v>64</v>
       </c>
       <c r="C76" s="1">
-        <v>44978.503472222219</v>
+        <v>43517.503472222219</v>
       </c>
       <c r="D76">
         <v>-48.99495494</v>
@@ -4313,10 +4316,10 @@
         <v>101</v>
       </c>
       <c r="G76" t="s">
-        <v>155</v>
+        <v>169</v>
       </c>
       <c r="H76" s="1">
-        <v>44978.621527777781</v>
+        <v>43517.621527777781</v>
       </c>
       <c r="I76">
         <v>-48.993211109999997</v>
@@ -4333,13 +4336,13 @@
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>156</v>
+        <v>81</v>
       </c>
       <c r="B77" t="s">
-        <v>145</v>
+        <v>76</v>
       </c>
       <c r="C77" s="1">
-        <v>44979.375</v>
+        <v>43518.375</v>
       </c>
       <c r="D77">
         <v>-48.993160830000001</v>
@@ -4351,10 +4354,10 @@
         <v>105</v>
       </c>
       <c r="G77" t="s">
-        <v>157</v>
+        <v>170</v>
       </c>
       <c r="H77" s="1">
-        <v>44979.416666666664</v>
+        <v>43518.416666666664</v>
       </c>
       <c r="I77">
         <v>-48.99355911</v>
@@ -4363,7 +4366,7 @@
         <v>-22.764021499999998</v>
       </c>
       <c r="K77" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="L77">
         <v>45</v>
@@ -4371,13 +4374,13 @@
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>158</v>
+        <v>82</v>
       </c>
       <c r="B78" t="s">
-        <v>153</v>
+        <v>80</v>
       </c>
       <c r="C78" s="1">
-        <v>44979.59375</v>
+        <v>43518.59375</v>
       </c>
       <c r="D78">
         <v>-48.994137729999998</v>
@@ -4389,10 +4392,10 @@
         <v>108</v>
       </c>
       <c r="G78" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="H78" s="1">
-        <v>44979.715277777781</v>
+        <v>43518.715277777781</v>
       </c>
       <c r="I78">
         <v>-48.995849300000003</v>
@@ -4409,13 +4412,13 @@
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>158</v>
+        <v>82</v>
       </c>
       <c r="B79" t="s">
         <v>13</v>
       </c>
       <c r="C79" s="1">
-        <v>44979.638888888891</v>
+        <v>43518.638888888891</v>
       </c>
       <c r="D79">
         <v>-48.994181480000002</v>
@@ -4427,10 +4430,10 @@
         <v>110</v>
       </c>
       <c r="G79" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="H79" s="1">
-        <v>44979.715277777781</v>
+        <v>43518.715277777781</v>
       </c>
       <c r="I79">
         <v>-48.995849300000003</v>
@@ -4447,13 +4450,13 @@
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>161</v>
+        <v>83</v>
       </c>
       <c r="B80" t="s">
-        <v>162</v>
+        <v>84</v>
       </c>
       <c r="C80" s="1">
-        <v>45022.527777777781</v>
+        <v>43561.527777777781</v>
       </c>
       <c r="D80">
         <v>-48.996477810000002</v>
@@ -4465,10 +4468,10 @@
         <v>112</v>
       </c>
       <c r="G80" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="H80" s="1">
-        <v>45022.618055555555</v>
+        <v>43561.618055555555</v>
       </c>
       <c r="I80">
         <v>-48.994985200000002</v>
@@ -4485,13 +4488,13 @@
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>164</v>
+        <v>85</v>
       </c>
       <c r="B81" t="s">
-        <v>162</v>
+        <v>84</v>
       </c>
       <c r="C81" s="1">
-        <v>45022.670138888891</v>
+        <v>43561.670138888891</v>
       </c>
       <c r="D81">
         <v>-48.99389429</v>
@@ -4503,10 +4506,10 @@
         <v>114</v>
       </c>
       <c r="G81" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="H81" s="1">
-        <v>45023.388888888891</v>
+        <v>43562.388888888891</v>
       </c>
       <c r="I81">
         <v>-48.995618530000002</v>
@@ -4523,13 +4526,13 @@
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>166</v>
+        <v>86</v>
       </c>
       <c r="B82" t="s">
-        <v>167</v>
+        <v>87</v>
       </c>
       <c r="C82" s="1">
-        <v>45023.604166666664</v>
+        <v>43562.604166666664</v>
       </c>
       <c r="D82">
         <v>-48.994640189999998</v>
@@ -4541,10 +4544,10 @@
         <v>119</v>
       </c>
       <c r="G82" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="H82" s="1">
-        <v>45024.340277777781</v>
+        <v>43563.340277777781</v>
       </c>
       <c r="I82">
         <v>-48.993108370000002</v>
@@ -4561,13 +4564,13 @@
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>166</v>
+        <v>86</v>
       </c>
       <c r="B83" t="s">
-        <v>169</v>
+        <v>88</v>
       </c>
       <c r="C83" s="1">
-        <v>45023.670138888891</v>
+        <v>43562.670138888891</v>
       </c>
       <c r="D83">
         <v>-48.993818869999998</v>
@@ -4579,10 +4582,10 @@
         <v>120</v>
       </c>
       <c r="G83" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="H83" s="1">
-        <v>45024.340277777781</v>
+        <v>43563.340277777781</v>
       </c>
       <c r="I83">
         <v>-48.993108370000002</v>
@@ -4591,7 +4594,7 @@
         <v>-22.762153479999998</v>
       </c>
       <c r="K83" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="L83">
         <v>79</v>
@@ -4599,13 +4602,13 @@
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>171</v>
+        <v>89</v>
       </c>
       <c r="B84" t="s">
-        <v>167</v>
+        <v>87</v>
       </c>
       <c r="C84" s="1">
-        <v>45025.496527777781</v>
+        <v>43564.496527777781</v>
       </c>
       <c r="D84">
         <v>-48.995843809999997</v>
@@ -4617,10 +4620,10 @@
         <v>126</v>
       </c>
       <c r="G84" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="H84" s="1">
-        <v>45025.576388888891</v>
+        <v>43564.576388888891</v>
       </c>
       <c r="I84">
         <v>-48.996098879999998</v>
@@ -4637,13 +4640,13 @@
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>173</v>
+        <v>90</v>
       </c>
       <c r="B85" t="s">
-        <v>169</v>
+        <v>88</v>
       </c>
       <c r="C85" s="1">
-        <v>45025.565972222219</v>
+        <v>43564.565972222219</v>
       </c>
       <c r="D85">
         <v>-48.996109390000001</v>
@@ -4655,10 +4658,10 @@
         <v>127</v>
       </c>
       <c r="G85" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="H85" s="1">
-        <v>45025.680555555555</v>
+        <v>43564.680555555555</v>
       </c>
       <c r="I85">
         <v>-48.994567439999997</v>
@@ -4667,7 +4670,7 @@
         <v>-22.761506239999999</v>
       </c>
       <c r="K85" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="L85">
         <v>185</v>
@@ -4675,13 +4678,13 @@
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>173</v>
+        <v>90</v>
       </c>
       <c r="B86" t="s">
-        <v>167</v>
+        <v>87</v>
       </c>
       <c r="C86" s="1">
-        <v>45025.59375</v>
+        <v>43564.59375</v>
       </c>
       <c r="D86">
         <v>-48.996178299999997</v>
@@ -4693,10 +4696,10 @@
         <v>128</v>
       </c>
       <c r="G86" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="H86" s="1">
-        <v>45025.680555555555</v>
+        <v>43564.680555555555</v>
       </c>
       <c r="I86">
         <v>-48.994567439999997</v>
@@ -4713,13 +4716,13 @@
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>176</v>
+        <v>91</v>
       </c>
       <c r="B87" t="s">
-        <v>177</v>
+        <v>92</v>
       </c>
       <c r="C87" s="1">
-        <v>45029.631944444445</v>
+        <v>43568.631944444445</v>
       </c>
       <c r="D87">
         <v>-48.997669709999997</v>
@@ -4731,10 +4734,10 @@
         <v>134</v>
       </c>
       <c r="G87" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="H87" s="1">
-        <v>45029.697916666664</v>
+        <v>43568.697916666664</v>
       </c>
       <c r="I87">
         <v>-48.99638856</v>
@@ -4751,13 +4754,13 @@
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>176</v>
+        <v>91</v>
       </c>
       <c r="B88" t="s">
-        <v>179</v>
+        <v>93</v>
       </c>
       <c r="C88" s="1">
-        <v>45029.631944444445</v>
+        <v>43568.631944444445</v>
       </c>
       <c r="D88">
         <v>-48.997669709999997</v>
@@ -4769,10 +4772,10 @@
         <v>135</v>
       </c>
       <c r="G88" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H88" s="1">
-        <v>45029.697916666664</v>
+        <v>43568.697916666664</v>
       </c>
       <c r="I88">
         <v>-48.99638856</v>
@@ -4789,13 +4792,13 @@
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>181</v>
+        <v>94</v>
       </c>
       <c r="B89" t="s">
-        <v>169</v>
+        <v>88</v>
       </c>
       <c r="C89" s="1">
-        <v>45030.347222222219</v>
+        <v>43569.347222222219</v>
       </c>
       <c r="D89">
         <v>-48.9968918</v>
@@ -4810,7 +4813,7 @@
         <v>182</v>
       </c>
       <c r="H89" s="1">
-        <v>45030.402777777781</v>
+        <v>43569.402777777781</v>
       </c>
       <c r="I89">
         <v>-48.996458279999999</v>
@@ -4819,7 +4822,7 @@
         <v>-22.763005379999999</v>
       </c>
       <c r="K89" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="L89">
         <v>145</v>

</xml_diff>

<commit_message>
Rechecking Movement and seed dispersal data (month_id) for matching the timeframes of the siminputrow timeframes table
</commit_message>
<xml_diff>
--- a/Data/Seed_dispersal/Raw_SuzanoAnne_07d-04-2021_Seed-dispersal.xlsx
+++ b/Data/Seed_dispersal/Raw_SuzanoAnne_07d-04-2021_Seed-dispersal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Documentos\github\BLT_IBM-Model\Data\Seed_dispersal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C4C7FC-F896-4175-82F8-2EBF32F289C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E225C2C-9A62-4622-B6F4-F752297D3A12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="188">
   <si>
     <t>id_feces</t>
   </si>
@@ -569,6 +569,21 @@
   </si>
   <si>
     <t>SDSuzApr88</t>
+  </si>
+  <si>
+    <t>id_month</t>
+  </si>
+  <si>
+    <t>Sep</t>
+  </si>
+  <si>
+    <t>Dec</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>Apr</t>
   </si>
 </sst>
 </file>
@@ -1431,3400 +1446,3666 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L89"/>
+  <dimension ref="A1:M89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="5"/>
-    <col min="7" max="7" width="9.88671875" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="5"/>
+    <col min="8" max="8" width="9.88671875" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D2" s="1">
         <v>43352.489583333336</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>-48.995342430000001</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>-22.76231984</v>
       </c>
-      <c r="F2" s="5">
+      <c r="G2" s="5">
         <v>3</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>95</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <v>43352.618055555555</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>-48.993802109999997</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>-22.763020999999998</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>4</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>174</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D3" s="1">
         <v>43352.489583333336</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>-48.995342430000001</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>-22.76231984</v>
       </c>
-      <c r="F3" s="5">
+      <c r="G3" s="5">
         <v>3</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>96</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>43352.621527777781</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>-48.993657800000001</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>-22.763056809999998</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>5</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>189</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D4" s="1">
         <v>43352.489583333336</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>-48.995342430000001</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>-22.76231984</v>
       </c>
-      <c r="F4" s="5">
+      <c r="G4" s="5">
         <v>4</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>97</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <v>43352.618055555555</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>-48.993802109999997</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>-22.763020999999998</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>6</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>174</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" t="s">
+        <v>184</v>
+      </c>
+      <c r="D5" s="1">
         <v>43352.489583333336</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>-48.995342430000001</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>-22.76231984</v>
       </c>
-      <c r="F5" s="5">
+      <c r="G5" s="5">
         <v>4</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>98</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>43352.621527777781</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>-48.993657800000001</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>-22.763056809999998</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>5</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>189</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" t="s">
+        <v>184</v>
+      </c>
+      <c r="D6" s="1">
         <v>43352.538194444445</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>-48.994742870000003</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>-22.762396209999999</v>
       </c>
-      <c r="F6" s="5">
+      <c r="G6" s="5">
         <v>5</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>99</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <v>43352.618055555555</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>-48.993802109999997</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>-22.763020999999998</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>8</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" t="s">
+        <v>184</v>
+      </c>
+      <c r="D7" s="1">
         <v>43352.545138888891</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>-48.994703199999996</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>-22.762326340000001</v>
       </c>
-      <c r="F7" s="5">
+      <c r="G7" s="5">
         <v>6</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>100</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <v>43352.625</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>-48.993657800000001</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>-22.763056809999998</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>7</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" t="s">
+        <v>184</v>
+      </c>
+      <c r="D8" s="1">
         <v>43352.628472222219</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>-48.993657800000001</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>-22.763056809999998</v>
       </c>
-      <c r="F8" s="5">
+      <c r="G8" s="5">
         <v>7</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>101</v>
       </c>
-      <c r="H8" s="1">
+      <c r="I8" s="1">
         <v>43353.329861111109</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>-48.993224810000001</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>-22.763371159999998</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>7</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" t="s">
+        <v>184</v>
+      </c>
+      <c r="D9" s="1">
         <v>43352.631944444445</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>-48.993629319999997</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>-22.762979789999999</v>
       </c>
-      <c r="F9" s="5">
+      <c r="G9" s="5">
         <v>8</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>102</v>
       </c>
-      <c r="H9" s="1">
+      <c r="I9" s="1">
         <v>43353.333333333336</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>-48.993189200000003</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>-22.763272189999999</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>6</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" t="s">
+        <v>184</v>
+      </c>
+      <c r="D10" s="1">
         <v>43352.697916666664</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>-48.99354598</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>-22.76379815</v>
       </c>
-      <c r="F10" s="5">
+      <c r="G10" s="5">
         <v>9</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>103</v>
       </c>
-      <c r="H10" s="1">
+      <c r="I10" s="1">
         <v>43353.34375</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>-48.993125310000003</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>-22.763123539999999</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>4</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" t="s">
+        <v>184</v>
+      </c>
+      <c r="D11" s="1">
         <v>43352.697916666664</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>-48.99354598</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>-22.76379815</v>
       </c>
-      <c r="F11" s="5">
+      <c r="G11" s="5">
         <v>9</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>104</v>
       </c>
-      <c r="H11" s="1">
+      <c r="I11" s="1">
         <v>43353.357638888891</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>-48.993201130000003</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>-22.76309273</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>5</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
       <c r="B12" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" t="s">
+        <v>184</v>
+      </c>
+      <c r="D12" s="1">
         <v>43353.583333333336</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>-48.993023960000002</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>-22.763631</v>
       </c>
-      <c r="F12" s="5">
+      <c r="G12" s="5">
         <v>15</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>105</v>
       </c>
-      <c r="H12" s="1">
+      <c r="I12" s="1">
         <v>43353.663194444445</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>-48.993141659999999</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>-22.76392164</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>4</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
       <c r="B13" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" t="s">
+        <v>184</v>
+      </c>
+      <c r="D13" s="1">
         <v>43353.677083333336</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>-48.993198679999999</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>-22.763752140000001</v>
       </c>
-      <c r="F13" s="5">
+      <c r="G13" s="5">
         <v>17</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>106</v>
       </c>
-      <c r="H13" s="1">
+      <c r="I13" s="1">
         <v>43354.319444444445</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>-48.99342867</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>-22.76393427</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>2</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>25</v>
       </c>
       <c r="B14" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" t="s">
+        <v>184</v>
+      </c>
+      <c r="D14" s="1">
         <v>43354.486111111109</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>-48.99264367</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>-22.764722849999998</v>
       </c>
-      <c r="F14" s="5">
+      <c r="G14" s="5">
         <v>21</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>107</v>
       </c>
-      <c r="H14" s="1">
+      <c r="I14" s="1">
         <v>43354.569444444445</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>-48.992404180000001</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>-22.76405978</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>3</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>27</v>
       </c>
       <c r="B15" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" t="s">
+        <v>184</v>
+      </c>
+      <c r="D15" s="1">
         <v>43354.496527777781</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>-48.992633949999998</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>-22.764634359999999</v>
       </c>
-      <c r="F15" s="5">
+      <c r="G15" s="5">
         <v>22</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>108</v>
       </c>
-      <c r="H15" s="1">
+      <c r="I15" s="1">
         <v>43354.59375</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>-48.99268833</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>-22.76403766</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>29</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>27</v>
       </c>
       <c r="B16" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" t="s">
+        <v>184</v>
+      </c>
+      <c r="D16" s="1">
         <v>43354.5625</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>-48.992292229999997</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>-22.764116000000001</v>
       </c>
-      <c r="F16" s="5">
+      <c r="G16" s="5">
         <v>23</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>109</v>
       </c>
-      <c r="H16" s="1">
+      <c r="I16" s="1">
         <v>43354.59375</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>-48.99268833</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>-22.76403766</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>5</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>31</v>
       </c>
       <c r="B17" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" t="s">
+        <v>184</v>
+      </c>
+      <c r="D17" s="1">
         <v>43354.5625</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>-48.992292229999997</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>-22.764116000000001</v>
       </c>
-      <c r="F17" s="5">
+      <c r="G17" s="5">
         <v>23</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>110</v>
       </c>
-      <c r="H17" s="1">
+      <c r="I17" s="1">
         <v>43354.607638888891</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>-48.99278588</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>-22.763960269999998</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <v>4</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>27</v>
       </c>
       <c r="B18" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" t="s">
+        <v>184</v>
+      </c>
+      <c r="D18" s="1">
         <v>43354.576388888891</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>-48.992552459999999</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>-22.763985129999998</v>
       </c>
-      <c r="F18" s="5">
+      <c r="G18" s="5">
         <v>24</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>111</v>
       </c>
-      <c r="H18" s="1">
+      <c r="I18" s="1">
         <v>43354.59375</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>-48.99268833</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>-22.76403766</v>
       </c>
-      <c r="K18">
+      <c r="L18">
         <v>6</v>
       </c>
-      <c r="L18">
+      <c r="M18">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>33</v>
       </c>
       <c r="B19" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" t="s">
+        <v>184</v>
+      </c>
+      <c r="D19" s="1">
         <v>43354.576388888891</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>-48.99261327</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>-22.764015010000001</v>
       </c>
-      <c r="F19" s="5">
+      <c r="G19" s="5">
         <v>25</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>112</v>
       </c>
-      <c r="H19" s="1">
+      <c r="I19" s="1">
         <v>43354.680555555555</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>-48.993309009999997</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>-22.762503290000001</v>
       </c>
-      <c r="K19">
+      <c r="L19">
         <v>5</v>
       </c>
-      <c r="L19">
+      <c r="M19">
         <v>171</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>34</v>
       </c>
       <c r="B20" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" t="s">
+        <v>184</v>
+      </c>
+      <c r="D20" s="1">
         <v>43355.340277777781</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>-48.993463769999998</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>-22.762113660000001</v>
       </c>
-      <c r="F20" s="5">
+      <c r="G20" s="5">
         <v>29</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>113</v>
       </c>
-      <c r="H20" s="1">
+      <c r="I20" s="1">
         <v>43355.420138888891</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>-48.993868999999997</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>-22.7615081</v>
       </c>
-      <c r="K20">
+      <c r="L20">
         <v>5</v>
       </c>
-      <c r="L20">
+      <c r="M20">
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>35</v>
       </c>
       <c r="B21" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" t="s">
+        <v>184</v>
+      </c>
+      <c r="D21" s="1">
         <v>43355.340277777781</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>-48.993463769999998</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>-22.762113660000001</v>
       </c>
-      <c r="F21" s="5">
+      <c r="G21" s="5">
         <v>29</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>114</v>
       </c>
-      <c r="H21" s="1">
+      <c r="I21" s="1">
         <v>43355.430555555555</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>-48.993927810000002</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <v>-22.761594039999999</v>
       </c>
-      <c r="K21">
+      <c r="L21">
         <v>6</v>
       </c>
-      <c r="L21">
+      <c r="M21">
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>36</v>
       </c>
       <c r="B22" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" t="s">
+        <v>184</v>
+      </c>
+      <c r="D22" s="1">
         <v>43355.46875</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>-48.994121270000001</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>-22.761856649999999</v>
       </c>
-      <c r="F22" s="5">
+      <c r="G22" s="5">
         <v>30</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>115</v>
       </c>
-      <c r="H22" s="1">
+      <c r="I22" s="1">
         <v>43355.579861111109</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>-48.993888750000004</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <v>-22.7630537</v>
       </c>
-      <c r="K22">
+      <c r="L22">
         <v>7</v>
       </c>
-      <c r="L22">
+      <c r="M22">
         <v>125</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>38</v>
       </c>
       <c r="B23" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" t="s">
+        <v>184</v>
+      </c>
+      <c r="D23" s="1">
         <v>43355.46875</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>-48.994121270000001</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>-22.761856649999999</v>
       </c>
-      <c r="F23" s="5">
+      <c r="G23" s="5">
         <v>30</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>116</v>
       </c>
-      <c r="H23" s="1">
+      <c r="I23" s="1">
         <v>43355.586805555555</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>-48.993740500000001</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <v>-22.763368140000001</v>
       </c>
-      <c r="K23">
+      <c r="L23">
         <v>8</v>
       </c>
-      <c r="L23">
+      <c r="M23">
         <v>160</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>36</v>
       </c>
       <c r="B24" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" t="s">
+        <v>184</v>
+      </c>
+      <c r="D24" s="1">
         <v>43355.479166666664</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>-48.994082329999998</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>-22.76190708</v>
       </c>
-      <c r="F24" s="5">
+      <c r="G24" s="5">
         <v>31</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>117</v>
       </c>
-      <c r="H24" s="1">
+      <c r="I24" s="1">
         <v>43355.579861111109</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>-48.993888750000004</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>-22.7630537</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>29</v>
       </c>
-      <c r="L24">
+      <c r="M24">
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>38</v>
       </c>
       <c r="B25" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" t="s">
+        <v>184</v>
+      </c>
+      <c r="D25" s="1">
         <v>43355.479166666664</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>-48.994082329999998</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>-22.76190708</v>
       </c>
-      <c r="F25" s="5">
+      <c r="G25" s="5">
         <v>31</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>118</v>
       </c>
-      <c r="H25" s="1">
+      <c r="I25" s="1">
         <v>43355.586805555555</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <v>-48.993740500000001</v>
       </c>
-      <c r="J25">
+      <c r="K25">
         <v>-22.763368140000001</v>
       </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
         <v>29</v>
       </c>
-      <c r="L25">
+      <c r="M25">
         <v>154</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>39</v>
       </c>
       <c r="B26" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" t="s">
+        <v>185</v>
+      </c>
+      <c r="D26" s="1">
         <v>43441.309027777781</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>-48.993737889999998</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <v>-22.761462659999999</v>
       </c>
-      <c r="F26" s="5">
+      <c r="G26" s="5">
         <v>38</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>119</v>
       </c>
-      <c r="H26" s="1">
+      <c r="I26" s="1">
         <v>43441.399305555555</v>
       </c>
-      <c r="I26">
+      <c r="J26">
         <v>-48.994317559999999</v>
       </c>
-      <c r="J26">
+      <c r="K26">
         <v>-22.76166937</v>
       </c>
-      <c r="K26">
+      <c r="L26">
         <v>7</v>
       </c>
-      <c r="L26">
+      <c r="M26">
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>40</v>
       </c>
       <c r="B27" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" t="s">
+        <v>185</v>
+      </c>
+      <c r="D27" s="1">
         <v>43441.309027777781</v>
       </c>
-      <c r="D27">
+      <c r="E27">
         <v>-48.993737889999998</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>-22.761462659999999</v>
       </c>
-      <c r="F27" s="5">
+      <c r="G27" s="5">
         <v>38</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>120</v>
       </c>
-      <c r="H27" s="1">
+      <c r="I27" s="1">
         <v>43441.427083333336</v>
       </c>
-      <c r="I27">
+      <c r="J27">
         <v>-48.994461690000001</v>
       </c>
-      <c r="J27">
+      <c r="K27">
         <v>-22.762063139999999</v>
       </c>
-      <c r="K27">
+      <c r="L27">
         <v>8</v>
       </c>
-      <c r="L27">
+      <c r="M27">
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>41</v>
       </c>
       <c r="B28" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" t="s">
+        <v>185</v>
+      </c>
+      <c r="D28" s="1">
         <v>43441.399305555555</v>
       </c>
-      <c r="D28">
+      <c r="E28">
         <v>-48.994317559999999</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <v>-22.76166937</v>
       </c>
-      <c r="F28" s="5">
+      <c r="G28" s="5">
         <v>40</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>121</v>
       </c>
-      <c r="H28" s="1">
+      <c r="I28" s="1">
         <v>43441.482638888891</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <v>-48.995004940000001</v>
       </c>
-      <c r="J28">
+      <c r="K28">
         <v>-22.761896270000001</v>
       </c>
-      <c r="K28">
+      <c r="L28">
         <v>7</v>
       </c>
-      <c r="L28">
+      <c r="M28">
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>42</v>
       </c>
       <c r="B29" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29" t="s">
+        <v>185</v>
+      </c>
+      <c r="D29" s="1">
         <v>43441.399305555555</v>
       </c>
-      <c r="D29">
+      <c r="E29">
         <v>-48.994317559999999</v>
       </c>
-      <c r="E29">
+      <c r="F29">
         <v>-22.76166937</v>
       </c>
-      <c r="F29" s="5">
+      <c r="G29" s="5">
         <v>40</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>122</v>
       </c>
-      <c r="H29" s="1">
+      <c r="I29" s="1">
         <v>43441.510416666664</v>
       </c>
-      <c r="I29">
+      <c r="J29">
         <v>-48.995207010000001</v>
       </c>
-      <c r="J29">
+      <c r="K29">
         <v>-22.762457390000002</v>
       </c>
-      <c r="K29">
+      <c r="L29">
         <v>7</v>
       </c>
-      <c r="L29">
+      <c r="M29">
         <v>122</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>42</v>
       </c>
       <c r="B30" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" t="s">
+        <v>185</v>
+      </c>
+      <c r="D30" s="1">
         <v>43441.409722222219</v>
       </c>
-      <c r="D30">
+      <c r="E30">
         <v>-48.994269979999999</v>
       </c>
-      <c r="E30">
+      <c r="F30">
         <v>-22.761692409999998</v>
       </c>
-      <c r="F30" s="5">
+      <c r="G30" s="5">
         <v>41</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>123</v>
       </c>
-      <c r="H30" s="1">
+      <c r="I30" s="1">
         <v>43441.510416666664</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <v>-48.995207010000001</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <v>-22.762457390000002</v>
       </c>
-      <c r="K30">
+      <c r="L30">
         <v>7</v>
       </c>
-      <c r="L30">
+      <c r="M30">
         <v>124</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>43</v>
       </c>
       <c r="B31" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" t="s">
+        <v>185</v>
+      </c>
+      <c r="D31" s="1">
         <v>43441.510416666664</v>
       </c>
-      <c r="D31">
+      <c r="E31">
         <v>-48.995207010000001</v>
       </c>
-      <c r="E31">
+      <c r="F31">
         <v>-22.762457390000002</v>
       </c>
-      <c r="F31" s="5">
+      <c r="G31" s="5">
         <v>44</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>124</v>
       </c>
-      <c r="H31" s="1">
+      <c r="I31" s="1">
         <v>43441.572916666664</v>
       </c>
-      <c r="I31">
+      <c r="J31">
         <v>-48.99460165</v>
       </c>
-      <c r="J31">
+      <c r="K31">
         <v>-22.762502099999999</v>
       </c>
-      <c r="K31">
+      <c r="L31">
         <v>7</v>
       </c>
-      <c r="L31">
+      <c r="M31">
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>44</v>
       </c>
       <c r="B32" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32" t="s">
+        <v>185</v>
+      </c>
+      <c r="D32" s="1">
         <v>43441.510416666664</v>
       </c>
-      <c r="D32">
+      <c r="E32">
         <v>-48.995207010000001</v>
       </c>
-      <c r="E32">
+      <c r="F32">
         <v>-22.762457390000002</v>
       </c>
-      <c r="F32" s="5">
+      <c r="G32" s="5">
         <v>44</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>125</v>
       </c>
-      <c r="H32" s="1">
+      <c r="I32" s="1">
         <v>43441.583333333336</v>
       </c>
-      <c r="I32">
+      <c r="J32">
         <v>-48.994500739999999</v>
       </c>
-      <c r="J32">
+      <c r="K32">
         <v>-22.762470029999999</v>
       </c>
-      <c r="K32">
+      <c r="L32">
         <v>6</v>
       </c>
-      <c r="L32">
+      <c r="M32">
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>45</v>
       </c>
       <c r="B33" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" t="s">
+        <v>185</v>
+      </c>
+      <c r="D33" s="1">
         <v>43441.510416666664</v>
       </c>
-      <c r="D33">
+      <c r="E33">
         <v>-48.995207010000001</v>
       </c>
-      <c r="E33">
+      <c r="F33">
         <v>-22.762457390000002</v>
       </c>
-      <c r="F33" s="5">
+      <c r="G33" s="5">
         <v>44</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>126</v>
       </c>
-      <c r="H33" s="1">
+      <c r="I33" s="1">
         <v>43441.600694444445</v>
       </c>
-      <c r="I33">
+      <c r="J33">
         <v>-48.994441049999999</v>
       </c>
-      <c r="J33">
+      <c r="K33">
         <v>-22.762506250000001</v>
       </c>
-      <c r="K33">
+      <c r="L33">
         <v>7</v>
       </c>
-      <c r="L33">
+      <c r="M33">
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>43</v>
       </c>
       <c r="B34" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C34" t="s">
+        <v>185</v>
+      </c>
+      <c r="D34" s="1">
         <v>43441.520833333336</v>
       </c>
-      <c r="D34">
+      <c r="E34">
         <v>-48.995207010000001</v>
       </c>
-      <c r="E34">
+      <c r="F34">
         <v>-22.762457390000002</v>
       </c>
-      <c r="F34" s="5">
+      <c r="G34" s="5">
         <v>45</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>127</v>
       </c>
-      <c r="H34" s="1">
+      <c r="I34" s="1">
         <v>43441.572916666664</v>
       </c>
-      <c r="I34">
+      <c r="J34">
         <v>-48.99460165</v>
       </c>
-      <c r="J34">
+      <c r="K34">
         <v>-22.762502099999999</v>
       </c>
-      <c r="K34">
+      <c r="L34">
         <v>32</v>
       </c>
-      <c r="L34">
+      <c r="M34">
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>44</v>
       </c>
       <c r="B35" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" t="s">
+        <v>185</v>
+      </c>
+      <c r="D35" s="1">
         <v>43441.520833333336</v>
       </c>
-      <c r="D35">
+      <c r="E35">
         <v>-48.995207010000001</v>
       </c>
-      <c r="E35">
+      <c r="F35">
         <v>-22.762457390000002</v>
       </c>
-      <c r="F35" s="5">
+      <c r="G35" s="5">
         <v>45</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
         <v>128</v>
       </c>
-      <c r="H35" s="1">
+      <c r="I35" s="1">
         <v>43441.583333333336</v>
       </c>
-      <c r="I35">
+      <c r="J35">
         <v>-48.994500739999999</v>
       </c>
-      <c r="J35">
+      <c r="K35">
         <v>-22.762470029999999</v>
       </c>
-      <c r="K35">
+      <c r="L35">
         <v>44</v>
       </c>
-      <c r="L35">
+      <c r="M35">
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>45</v>
       </c>
       <c r="B36" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" t="s">
+        <v>185</v>
+      </c>
+      <c r="D36" s="1">
         <v>43441.520833333336</v>
       </c>
-      <c r="D36">
+      <c r="E36">
         <v>-48.995207010000001</v>
       </c>
-      <c r="E36">
+      <c r="F36">
         <v>-22.762457390000002</v>
       </c>
-      <c r="F36" s="5">
+      <c r="G36" s="5">
         <v>45</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
         <v>129</v>
       </c>
-      <c r="H36" s="1">
+      <c r="I36" s="1">
         <v>43441.600694444445</v>
       </c>
-      <c r="I36">
+      <c r="J36">
         <v>-48.994441049999999</v>
       </c>
-      <c r="J36">
+      <c r="K36">
         <v>-22.762506250000001</v>
       </c>
-      <c r="K36">
+      <c r="L36">
         <v>28</v>
       </c>
-      <c r="L36">
+      <c r="M36">
         <v>79</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>47</v>
       </c>
       <c r="B37" t="s">
         <v>13</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C37" t="s">
+        <v>185</v>
+      </c>
+      <c r="D37" s="1">
         <v>43441.635416666664</v>
       </c>
-      <c r="D37">
+      <c r="E37">
         <v>-48.994267729999997</v>
       </c>
-      <c r="E37">
+      <c r="F37">
         <v>-22.762512260000001</v>
       </c>
-      <c r="F37" s="5">
+      <c r="G37" s="5">
         <v>47</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>130</v>
       </c>
-      <c r="H37" s="1">
+      <c r="I37" s="1">
         <v>43441.725694444445</v>
       </c>
-      <c r="I37">
+      <c r="J37">
         <v>-48.993462010000002</v>
       </c>
-      <c r="J37">
+      <c r="K37">
         <v>-22.762905109999998</v>
       </c>
-      <c r="K37">
+      <c r="L37">
         <v>8</v>
       </c>
-      <c r="L37">
+      <c r="M37">
         <v>92</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>48</v>
       </c>
       <c r="B38" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C38" t="s">
+        <v>185</v>
+      </c>
+      <c r="D38" s="1">
         <v>43441.635416666664</v>
       </c>
-      <c r="D38">
+      <c r="E38">
         <v>-48.994267729999997</v>
       </c>
-      <c r="E38">
+      <c r="F38">
         <v>-22.762512260000001</v>
       </c>
-      <c r="F38" s="5">
+      <c r="G38" s="5">
         <v>47</v>
       </c>
-      <c r="G38" t="s">
+      <c r="H38" t="s">
         <v>131</v>
       </c>
-      <c r="H38" s="1">
+      <c r="I38" s="1">
         <v>43441.725694444445</v>
       </c>
-      <c r="I38">
+      <c r="J38">
         <v>-48.993462010000002</v>
       </c>
-      <c r="J38">
+      <c r="K38">
         <v>-22.762905109999998</v>
       </c>
-      <c r="K38">
+      <c r="L38">
         <v>7</v>
       </c>
-      <c r="L38">
+      <c r="M38">
         <v>92</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>49</v>
       </c>
       <c r="B39" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="1">
+      <c r="C39" t="s">
+        <v>185</v>
+      </c>
+      <c r="D39" s="1">
         <v>43441.711805555555</v>
       </c>
-      <c r="D39">
+      <c r="E39">
         <v>-48.993473360000003</v>
       </c>
-      <c r="E39">
+      <c r="F39">
         <v>-22.762759800000001</v>
       </c>
-      <c r="F39" s="5">
+      <c r="G39" s="5">
         <v>49</v>
       </c>
-      <c r="G39" t="s">
+      <c r="H39" t="s">
         <v>132</v>
       </c>
-      <c r="H39" s="1">
+      <c r="I39" s="1">
         <v>43442.315972222219</v>
       </c>
-      <c r="I39">
+      <c r="J39">
         <v>-48.993229880000001</v>
       </c>
-      <c r="J39">
+      <c r="K39">
         <v>-22.763354400000001</v>
       </c>
-      <c r="K39">
+      <c r="L39">
         <v>7</v>
       </c>
-      <c r="L39">
+      <c r="M39">
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>50</v>
       </c>
       <c r="B40" t="s">
         <v>13</v>
       </c>
-      <c r="C40" s="1">
+      <c r="C40" t="s">
+        <v>185</v>
+      </c>
+      <c r="D40" s="1">
         <v>43441.711805555555</v>
       </c>
-      <c r="D40">
+      <c r="E40">
         <v>-48.993473360000003</v>
       </c>
-      <c r="E40">
+      <c r="F40">
         <v>-22.762759800000001</v>
       </c>
-      <c r="F40" s="5">
+      <c r="G40" s="5">
         <v>49</v>
       </c>
-      <c r="G40" t="s">
+      <c r="H40" t="s">
         <v>133</v>
       </c>
-      <c r="H40" s="1">
+      <c r="I40" s="1">
         <v>43442.347222222219</v>
       </c>
-      <c r="I40">
+      <c r="J40">
         <v>-48.99376032</v>
       </c>
-      <c r="J40">
+      <c r="K40">
         <v>-22.763564939999998</v>
       </c>
-      <c r="K40">
+      <c r="L40">
         <v>7</v>
       </c>
-      <c r="L40">
+      <c r="M40">
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>51</v>
       </c>
       <c r="B41" t="s">
         <v>16</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C41" t="s">
+        <v>185</v>
+      </c>
+      <c r="D41" s="1">
         <v>43442.385416666664</v>
       </c>
-      <c r="D41">
+      <c r="E41">
         <v>-48.99397982</v>
       </c>
-      <c r="E41">
+      <c r="F41">
         <v>-22.763198110000001</v>
       </c>
-      <c r="F41" s="5">
+      <c r="G41" s="5">
         <v>50</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>134</v>
       </c>
-      <c r="H41" s="1">
+      <c r="I41" s="1">
         <v>43442.4375</v>
       </c>
-      <c r="I41">
+      <c r="J41">
         <v>-48.993346219999999</v>
       </c>
-      <c r="J41">
+      <c r="K41">
         <v>-22.762248419999999</v>
       </c>
-      <c r="K41">
+      <c r="L41">
         <v>7</v>
       </c>
-      <c r="L41">
+      <c r="M41">
         <v>117</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>52</v>
       </c>
       <c r="B42" t="s">
         <v>16</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C42" t="s">
+        <v>185</v>
+      </c>
+      <c r="D42" s="1">
         <v>43442.385416666664</v>
       </c>
-      <c r="D42">
+      <c r="E42">
         <v>-48.99397982</v>
       </c>
-      <c r="E42">
+      <c r="F42">
         <v>-22.763198110000001</v>
       </c>
-      <c r="F42" s="5">
+      <c r="G42" s="5">
         <v>50</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>135</v>
       </c>
-      <c r="H42" s="1">
+      <c r="I42" s="1">
         <v>43442.451388888891</v>
       </c>
-      <c r="I42">
+      <c r="J42">
         <v>-48.99379407</v>
       </c>
-      <c r="J42">
+      <c r="K42">
         <v>-22.76221335</v>
       </c>
-      <c r="K42">
+      <c r="L42">
         <v>7</v>
       </c>
-      <c r="L42">
+      <c r="M42">
         <v>103</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>51</v>
       </c>
       <c r="B43" t="s">
         <v>13</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43" t="s">
+        <v>185</v>
+      </c>
+      <c r="D43" s="1">
         <v>43442.413194444445</v>
       </c>
-      <c r="D43">
+      <c r="E43">
         <v>-48.993354500000002</v>
       </c>
-      <c r="E43">
+      <c r="F43">
         <v>-22.7626299</v>
       </c>
-      <c r="F43" s="5">
+      <c r="G43" s="5">
         <v>51</v>
       </c>
-      <c r="G43" t="s">
+      <c r="H43" t="s">
         <v>136</v>
       </c>
-      <c r="H43" s="1">
+      <c r="I43" s="1">
         <v>43442.4375</v>
       </c>
-      <c r="I43">
+      <c r="J43">
         <v>-48.993346219999999</v>
       </c>
-      <c r="J43">
+      <c r="K43">
         <v>-22.762248419999999</v>
       </c>
-      <c r="K43">
+      <c r="L43">
         <v>8</v>
       </c>
-      <c r="L43">
+      <c r="M43">
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>53</v>
       </c>
       <c r="B44" t="s">
         <v>54</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44" t="s">
+        <v>185</v>
+      </c>
+      <c r="D44" s="1">
         <v>43442.649305555555</v>
       </c>
-      <c r="D44">
+      <c r="E44">
         <v>-48.993572129999997</v>
       </c>
-      <c r="E44">
+      <c r="F44">
         <v>-22.76184804</v>
       </c>
-      <c r="F44" s="5">
+      <c r="G44" s="5">
         <v>54</v>
       </c>
-      <c r="G44" t="s">
+      <c r="H44" t="s">
         <v>137</v>
       </c>
-      <c r="H44" s="1">
+      <c r="I44" s="1">
         <v>43443.350694444445</v>
       </c>
-      <c r="I44">
+      <c r="J44">
         <v>-48.993904710000002</v>
       </c>
-      <c r="J44">
+      <c r="K44">
         <v>-22.763448019999998</v>
       </c>
-      <c r="K44">
+      <c r="L44">
         <v>6</v>
       </c>
-      <c r="L44">
+      <c r="M44">
         <v>168</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>55</v>
       </c>
       <c r="B45" t="s">
         <v>54</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45" t="s">
+        <v>185</v>
+      </c>
+      <c r="D45" s="1">
         <v>43442.666666666664</v>
       </c>
-      <c r="D45">
+      <c r="E45">
         <v>-48.993351590000003</v>
       </c>
-      <c r="E45">
+      <c r="F45">
         <v>-22.761768440000001</v>
       </c>
-      <c r="F45" s="5">
+      <c r="G45" s="5">
         <v>55</v>
       </c>
-      <c r="G45" t="s">
+      <c r="H45" t="s">
         <v>138</v>
       </c>
-      <c r="H45" s="1">
+      <c r="I45" s="1">
         <v>43443.350694444445</v>
       </c>
-      <c r="I45">
+      <c r="J45">
         <v>-48.993904710000002</v>
       </c>
-      <c r="J45">
+      <c r="K45">
         <v>-22.763448019999998</v>
       </c>
-      <c r="K45">
+      <c r="L45">
         <v>5</v>
       </c>
-      <c r="L45">
+      <c r="M45">
         <v>182</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>56</v>
       </c>
       <c r="B46" t="s">
         <v>13</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C46" t="s">
+        <v>185</v>
+      </c>
+      <c r="D46" s="1">
         <v>43443.548611111109</v>
       </c>
-      <c r="D46">
+      <c r="E46">
         <v>-48.995160329999997</v>
       </c>
-      <c r="E46">
+      <c r="F46">
         <v>-22.762197889999999</v>
       </c>
-      <c r="F46" s="5">
+      <c r="G46" s="5">
         <v>58</v>
       </c>
-      <c r="G46" t="s">
+      <c r="H46" t="s">
         <v>139</v>
       </c>
-      <c r="H46" s="1">
+      <c r="I46" s="1">
         <v>43443.614583333336</v>
       </c>
-      <c r="I46">
+      <c r="J46">
         <v>-48.993649730000001</v>
       </c>
-      <c r="J46">
+      <c r="K46">
         <v>-22.762384470000001</v>
       </c>
-      <c r="K46">
+      <c r="L46">
         <v>7</v>
       </c>
-      <c r="L46">
+      <c r="M46">
         <v>157</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>57</v>
       </c>
       <c r="B47" t="s">
         <v>13</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C47" t="s">
+        <v>185</v>
+      </c>
+      <c r="D47" s="1">
         <v>43443.548611111109</v>
       </c>
-      <c r="D47">
+      <c r="E47">
         <v>-48.995160329999997</v>
       </c>
-      <c r="E47">
+      <c r="F47">
         <v>-22.762197889999999</v>
       </c>
-      <c r="F47" s="5">
+      <c r="G47" s="5">
         <v>58</v>
       </c>
-      <c r="G47" t="s">
+      <c r="H47" t="s">
         <v>140</v>
       </c>
-      <c r="H47" s="1">
+      <c r="I47" s="1">
         <v>43443.642361111109</v>
       </c>
-      <c r="I47">
+      <c r="J47">
         <v>-48.99320908</v>
       </c>
-      <c r="J47">
+      <c r="K47">
         <v>-22.762343950000002</v>
       </c>
-      <c r="K47">
+      <c r="L47">
         <v>6</v>
       </c>
-      <c r="L47">
+      <c r="M47">
         <v>201</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>56</v>
       </c>
       <c r="B48" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="1">
+      <c r="C48" t="s">
+        <v>185</v>
+      </c>
+      <c r="D48" s="1">
         <v>43443.548611111109</v>
       </c>
-      <c r="D48">
+      <c r="E48">
         <v>-48.995160329999997</v>
       </c>
-      <c r="E48">
+      <c r="F48">
         <v>-22.762197889999999</v>
       </c>
-      <c r="F48" s="5">
+      <c r="G48" s="5">
         <v>59</v>
       </c>
-      <c r="G48" t="s">
+      <c r="H48" t="s">
         <v>141</v>
       </c>
-      <c r="H48" s="1">
+      <c r="I48" s="1">
         <v>43443.614583333336</v>
       </c>
-      <c r="I48">
+      <c r="J48">
         <v>-48.993649730000001</v>
       </c>
-      <c r="J48">
+      <c r="K48">
         <v>-22.762384470000001</v>
       </c>
-      <c r="K48">
+      <c r="L48">
         <v>33</v>
       </c>
-      <c r="L48">
+      <c r="M48">
         <v>157</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>57</v>
       </c>
       <c r="B49" t="s">
         <v>46</v>
       </c>
-      <c r="C49" s="1">
+      <c r="C49" t="s">
+        <v>185</v>
+      </c>
+      <c r="D49" s="1">
         <v>43443.548611111109</v>
       </c>
-      <c r="D49">
+      <c r="E49">
         <v>-48.995160329999997</v>
       </c>
-      <c r="E49">
+      <c r="F49">
         <v>-22.762197889999999</v>
       </c>
-      <c r="F49" s="5">
+      <c r="G49" s="5">
         <v>59</v>
       </c>
-      <c r="G49" t="s">
+      <c r="H49" t="s">
         <v>142</v>
       </c>
-      <c r="H49" s="1">
+      <c r="I49" s="1">
         <v>43443.642361111109</v>
       </c>
-      <c r="I49">
+      <c r="J49">
         <v>-48.99320908</v>
       </c>
-      <c r="J49">
+      <c r="K49">
         <v>-22.762343950000002</v>
       </c>
-      <c r="K49">
+      <c r="L49">
         <v>38</v>
       </c>
-      <c r="L49">
+      <c r="M49">
         <v>201</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>58</v>
       </c>
       <c r="B50" t="s">
         <v>16</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C50" t="s">
+        <v>185</v>
+      </c>
+      <c r="D50" s="1">
         <v>43444.444444444445</v>
       </c>
-      <c r="D50">
+      <c r="E50">
         <v>-48.99409824</v>
       </c>
-      <c r="E50">
+      <c r="F50">
         <v>-22.762251240000001</v>
       </c>
-      <c r="F50" s="5">
+      <c r="G50" s="5">
         <v>67</v>
       </c>
-      <c r="G50" t="s">
+      <c r="H50" t="s">
         <v>143</v>
       </c>
-      <c r="H50" s="1">
+      <c r="I50" s="1">
         <v>43444.503472222219</v>
       </c>
-      <c r="I50">
+      <c r="J50">
         <v>-48.994872350000001</v>
       </c>
-      <c r="J50">
+      <c r="K50">
         <v>-22.762063810000001</v>
       </c>
-      <c r="K50">
+      <c r="L50">
         <v>5</v>
       </c>
-      <c r="L50">
+      <c r="M50">
         <v>82</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>59</v>
       </c>
       <c r="B51" t="s">
         <v>16</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C51" t="s">
+        <v>185</v>
+      </c>
+      <c r="D51" s="1">
         <v>43444.444444444445</v>
       </c>
-      <c r="D51">
+      <c r="E51">
         <v>-48.99409824</v>
       </c>
-      <c r="E51">
+      <c r="F51">
         <v>-22.762251240000001</v>
       </c>
-      <c r="F51" s="5">
+      <c r="G51" s="5">
         <v>67</v>
       </c>
-      <c r="G51" t="s">
+      <c r="H51" t="s">
         <v>144</v>
       </c>
-      <c r="H51" s="1">
+      <c r="I51" s="1">
         <v>43444.538194444445</v>
       </c>
-      <c r="I51">
+      <c r="J51">
         <v>-48.994877449999997</v>
       </c>
-      <c r="J51">
+      <c r="K51">
         <v>-22.76198527</v>
       </c>
-      <c r="K51">
+      <c r="L51">
         <v>7</v>
       </c>
-      <c r="L51">
+      <c r="M51">
         <v>85</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>60</v>
       </c>
       <c r="B52" t="s">
         <v>46</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C52" t="s">
+        <v>185</v>
+      </c>
+      <c r="D52" s="1">
         <v>43445.524305555555</v>
       </c>
-      <c r="D52">
+      <c r="E52">
         <v>-48.996441760000003</v>
       </c>
-      <c r="E52">
+      <c r="F52">
         <v>-22.762240689999999</v>
       </c>
-      <c r="F52" s="5">
+      <c r="G52" s="5">
         <v>74</v>
       </c>
-      <c r="G52" t="s">
+      <c r="H52" t="s">
         <v>145</v>
       </c>
-      <c r="H52" s="1">
+      <c r="I52" s="1">
         <v>43445.663194444445</v>
       </c>
-      <c r="I52">
+      <c r="J52">
         <v>-48.99419743</v>
       </c>
-      <c r="J52">
+      <c r="K52">
         <v>-22.762391869999998</v>
       </c>
-      <c r="K52">
+      <c r="L52">
         <v>45</v>
       </c>
-      <c r="L52">
+      <c r="M52">
         <v>231</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>60</v>
       </c>
       <c r="B53" t="s">
         <v>16</v>
       </c>
-      <c r="C53" s="1">
+      <c r="C53" t="s">
+        <v>185</v>
+      </c>
+      <c r="D53" s="1">
         <v>43445.555555555555</v>
       </c>
-      <c r="D53">
+      <c r="E53">
         <v>-48.996403870000002</v>
       </c>
-      <c r="E53">
+      <c r="F53">
         <v>-22.7626639</v>
       </c>
-      <c r="F53" s="5">
+      <c r="G53" s="5">
         <v>75</v>
       </c>
-      <c r="G53" t="s">
+      <c r="H53" t="s">
         <v>146</v>
       </c>
-      <c r="H53" s="1">
+      <c r="I53" s="1">
         <v>43445.663194444445</v>
       </c>
-      <c r="I53">
+      <c r="J53">
         <v>-48.99419743</v>
       </c>
-      <c r="J53">
+      <c r="K53">
         <v>-22.762391869999998</v>
       </c>
-      <c r="K53">
+      <c r="L53">
         <v>7</v>
       </c>
-      <c r="L53">
+      <c r="M53">
         <v>229</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>61</v>
       </c>
       <c r="B54" t="s">
         <v>16</v>
       </c>
-      <c r="C54" s="1">
+      <c r="C54" t="s">
+        <v>185</v>
+      </c>
+      <c r="D54" s="1">
         <v>43446.447916666664</v>
       </c>
-      <c r="D54">
+      <c r="E54">
         <v>-48.995943330000003</v>
       </c>
-      <c r="E54">
+      <c r="F54">
         <v>-22.762665089999999</v>
       </c>
-      <c r="F54" s="5">
+      <c r="G54" s="5">
         <v>77</v>
       </c>
-      <c r="G54" t="s">
+      <c r="H54" t="s">
         <v>147</v>
       </c>
-      <c r="H54" s="1">
+      <c r="I54" s="1">
         <v>43446.46875</v>
       </c>
-      <c r="I54">
+      <c r="J54">
         <v>-48.996503789999998</v>
       </c>
-      <c r="J54">
+      <c r="K54">
         <v>-22.76279864</v>
       </c>
-      <c r="K54">
+      <c r="L54">
         <v>6</v>
       </c>
-      <c r="L54">
+      <c r="M54">
         <v>59</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>61</v>
       </c>
       <c r="B55" t="s">
         <v>13</v>
       </c>
-      <c r="C55" s="1">
+      <c r="C55" t="s">
+        <v>185</v>
+      </c>
+      <c r="D55" s="1">
         <v>43446.447916666664</v>
       </c>
-      <c r="D55">
+      <c r="E55">
         <v>-48.995943330000003</v>
       </c>
-      <c r="E55">
+      <c r="F55">
         <v>-22.762665089999999</v>
       </c>
-      <c r="F55" s="5">
+      <c r="G55" s="5">
         <v>78</v>
       </c>
-      <c r="G55" t="s">
+      <c r="H55" t="s">
         <v>148</v>
       </c>
-      <c r="H55" s="1">
+      <c r="I55" s="1">
         <v>43446.46875</v>
       </c>
-      <c r="I55">
+      <c r="J55">
         <v>-48.996503789999998</v>
       </c>
-      <c r="J55">
+      <c r="K55">
         <v>-22.76279864</v>
       </c>
-      <c r="K55">
+      <c r="L55">
         <v>7</v>
       </c>
-      <c r="L55">
+      <c r="M55">
         <v>59</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>62</v>
       </c>
       <c r="B56" t="s">
         <v>16</v>
       </c>
-      <c r="C56" s="1">
+      <c r="C56" t="s">
+        <v>185</v>
+      </c>
+      <c r="D56" s="1">
         <v>43446.451388888891</v>
       </c>
-      <c r="D56">
+      <c r="E56">
         <v>-48.995943330000003</v>
       </c>
-      <c r="E56">
+      <c r="F56">
         <v>-22.762665089999999</v>
       </c>
-      <c r="F56" s="5">
+      <c r="G56" s="5">
         <v>77</v>
       </c>
-      <c r="G56" t="s">
+      <c r="H56" t="s">
         <v>149</v>
       </c>
-      <c r="H56" s="1">
+      <c r="I56" s="1">
         <v>43446.482638888891</v>
       </c>
-      <c r="I56">
+      <c r="J56">
         <v>-48.99659406</v>
       </c>
-      <c r="J56">
+      <c r="K56">
         <v>-22.762968399999998</v>
       </c>
-      <c r="K56">
+      <c r="L56">
         <v>7</v>
       </c>
-      <c r="L56">
+      <c r="M56">
         <v>74</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>62</v>
       </c>
       <c r="B57" t="s">
         <v>13</v>
       </c>
-      <c r="C57" s="1">
+      <c r="C57" t="s">
+        <v>185</v>
+      </c>
+      <c r="D57" s="1">
         <v>43446.451388888891</v>
       </c>
-      <c r="D57">
+      <c r="E57">
         <v>-48.995943330000003</v>
       </c>
-      <c r="E57">
+      <c r="F57">
         <v>-22.762665089999999</v>
       </c>
-      <c r="F57" s="5">
+      <c r="G57" s="5">
         <v>78</v>
       </c>
-      <c r="G57" t="s">
+      <c r="H57" t="s">
         <v>150</v>
       </c>
-      <c r="H57" s="1">
+      <c r="I57" s="1">
         <v>43446.482638888891</v>
       </c>
-      <c r="I57">
+      <c r="J57">
         <v>-48.99659406</v>
       </c>
-      <c r="J57">
+      <c r="K57">
         <v>-22.762968399999998</v>
       </c>
-      <c r="K57">
+      <c r="L57">
         <v>6</v>
       </c>
-      <c r="L57">
+      <c r="M57">
         <v>74</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>63</v>
       </c>
       <c r="B58" t="s">
         <v>64</v>
       </c>
-      <c r="C58" s="1">
+      <c r="C58" t="s">
+        <v>186</v>
+      </c>
+      <c r="D58" s="1">
         <v>43515.357638888891</v>
       </c>
-      <c r="D58">
+      <c r="E58">
         <v>-48.995732449999998</v>
       </c>
-      <c r="E58">
+      <c r="F58">
         <v>-22.76370313</v>
       </c>
-      <c r="F58" s="5">
+      <c r="G58" s="5">
         <v>81</v>
       </c>
-      <c r="G58" t="s">
+      <c r="H58" t="s">
         <v>151</v>
       </c>
-      <c r="H58" s="1">
+      <c r="I58" s="1">
         <v>43515.4375</v>
       </c>
-      <c r="I58">
+      <c r="J58">
         <v>-48.997744060000002</v>
       </c>
-      <c r="J58">
+      <c r="K58">
         <v>-22.763591120000001</v>
       </c>
-      <c r="K58">
+      <c r="L58">
         <v>4</v>
       </c>
-      <c r="L58">
+      <c r="M58">
         <v>207</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>65</v>
       </c>
       <c r="B59" t="s">
         <v>64</v>
       </c>
-      <c r="C59" s="1">
+      <c r="C59" t="s">
+        <v>186</v>
+      </c>
+      <c r="D59" s="1">
         <v>43515.357638888891</v>
       </c>
-      <c r="D59">
+      <c r="E59">
         <v>-48.995732449999998</v>
       </c>
-      <c r="E59">
+      <c r="F59">
         <v>-22.76370313</v>
       </c>
-      <c r="F59" s="5">
+      <c r="G59" s="5">
         <v>81</v>
       </c>
-      <c r="G59" t="s">
+      <c r="H59" t="s">
         <v>152</v>
       </c>
-      <c r="H59" s="1">
+      <c r="I59" s="1">
         <v>43515.444444444445</v>
       </c>
-      <c r="I59">
+      <c r="J59">
         <v>-48.997904830000003</v>
       </c>
-      <c r="J59">
+      <c r="K59">
         <v>-22.763545780000001</v>
       </c>
-      <c r="K59">
+      <c r="L59">
         <v>5</v>
       </c>
-      <c r="L59">
+      <c r="M59">
         <v>223</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>63</v>
       </c>
       <c r="B60" t="s">
         <v>66</v>
       </c>
-      <c r="C60" s="1">
+      <c r="C60" t="s">
+        <v>186</v>
+      </c>
+      <c r="D60" s="1">
         <v>43515.364583333336</v>
       </c>
-      <c r="D60">
+      <c r="E60">
         <v>-48.995850730000001</v>
       </c>
-      <c r="E60">
+      <c r="F60">
         <v>-22.763700539999999</v>
       </c>
-      <c r="F60" s="5">
+      <c r="G60" s="5">
         <v>82</v>
       </c>
-      <c r="G60" t="s">
+      <c r="H60" t="s">
         <v>153</v>
       </c>
-      <c r="H60" s="1">
+      <c r="I60" s="1">
         <v>43515.4375</v>
       </c>
-      <c r="I60">
+      <c r="J60">
         <v>-48.997744060000002</v>
       </c>
-      <c r="J60">
+      <c r="K60">
         <v>-22.763591120000001</v>
       </c>
-      <c r="K60">
+      <c r="L60">
         <v>2</v>
       </c>
-      <c r="L60">
+      <c r="M60">
         <v>295</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>65</v>
       </c>
       <c r="B61" t="s">
         <v>66</v>
       </c>
-      <c r="C61" s="1">
+      <c r="C61" t="s">
+        <v>186</v>
+      </c>
+      <c r="D61" s="1">
         <v>43515.364583333336</v>
       </c>
-      <c r="D61">
+      <c r="E61">
         <v>-48.995850730000001</v>
       </c>
-      <c r="E61">
+      <c r="F61">
         <v>-22.763700539999999</v>
       </c>
-      <c r="F61" s="5">
+      <c r="G61" s="5">
         <v>82</v>
       </c>
-      <c r="G61" t="s">
+      <c r="H61" t="s">
         <v>154</v>
       </c>
-      <c r="H61" s="1">
+      <c r="I61" s="1">
         <v>43515.444444444445</v>
       </c>
-      <c r="I61">
+      <c r="J61">
         <v>-48.997904830000003</v>
       </c>
-      <c r="J61">
+      <c r="K61">
         <v>-22.763545780000001</v>
       </c>
-      <c r="K61">
+      <c r="L61">
         <v>3</v>
       </c>
-      <c r="L61">
+      <c r="M61">
         <v>212</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>67</v>
       </c>
       <c r="B62" t="s">
         <v>66</v>
       </c>
-      <c r="C62" s="1">
+      <c r="C62" t="s">
+        <v>186</v>
+      </c>
+      <c r="D62" s="1">
         <v>43515.454861111109</v>
       </c>
-      <c r="D62">
+      <c r="E62">
         <v>-48.997605819999997</v>
       </c>
-      <c r="E62">
+      <c r="F62">
         <v>-22.763487099999999</v>
       </c>
-      <c r="F62" s="5">
+      <c r="G62" s="5">
         <v>83</v>
       </c>
-      <c r="G62" t="s">
+      <c r="H62" t="s">
         <v>155</v>
       </c>
-      <c r="H62" s="1">
+      <c r="I62" s="1">
         <v>43515.552083333336</v>
       </c>
-      <c r="I62">
+      <c r="J62">
         <v>-48.998115480000003</v>
       </c>
-      <c r="J62">
+      <c r="K62">
         <v>-22.764625290000001</v>
       </c>
-      <c r="K62">
+      <c r="L62">
         <v>3</v>
       </c>
-      <c r="L62">
+      <c r="M62">
         <v>128</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>68</v>
       </c>
       <c r="B63" t="s">
         <v>64</v>
       </c>
-      <c r="C63" s="1">
+      <c r="C63" t="s">
+        <v>186</v>
+      </c>
+      <c r="D63" s="1">
         <v>43515.472222222219</v>
       </c>
-      <c r="D63">
+      <c r="E63">
         <v>-48.997469240000001</v>
       </c>
-      <c r="E63">
+      <c r="F63">
         <v>-22.763606809999999</v>
       </c>
-      <c r="F63" s="5">
+      <c r="G63" s="5">
         <v>84</v>
       </c>
-      <c r="G63" t="s">
+      <c r="H63" t="s">
         <v>156</v>
       </c>
-      <c r="H63" s="1">
+      <c r="I63" s="1">
         <v>43515.579861111109</v>
       </c>
-      <c r="I63">
+      <c r="J63">
         <v>-48.997983300000001</v>
       </c>
-      <c r="J63">
+      <c r="K63">
         <v>-22.76469312</v>
       </c>
-      <c r="K63">
+      <c r="L63">
         <v>5</v>
       </c>
-      <c r="L63">
+      <c r="M63">
         <v>124</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>69</v>
       </c>
       <c r="B64" t="s">
         <v>66</v>
       </c>
-      <c r="C64" s="1">
+      <c r="C64" t="s">
+        <v>186</v>
+      </c>
+      <c r="D64" s="1">
         <v>43515.552083333336</v>
       </c>
-      <c r="D64">
+      <c r="E64">
         <v>-48.998115480000003</v>
       </c>
-      <c r="E64">
+      <c r="F64">
         <v>-22.764625290000001</v>
       </c>
-      <c r="F64" s="5">
+      <c r="G64" s="5">
         <v>86</v>
       </c>
-      <c r="G64" t="s">
+      <c r="H64" t="s">
         <v>157</v>
       </c>
-      <c r="H64" s="1">
+      <c r="I64" s="1">
         <v>43515.631944444445</v>
       </c>
-      <c r="I64">
+      <c r="J64">
         <v>-48.997880790000004</v>
       </c>
-      <c r="J64">
+      <c r="K64">
         <v>-22.764848860000001</v>
       </c>
-      <c r="K64">
+      <c r="L64">
         <v>2</v>
       </c>
-      <c r="L64">
+      <c r="M64">
         <v>33</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>70</v>
       </c>
       <c r="B65" t="s">
         <v>71</v>
       </c>
-      <c r="C65" s="1">
+      <c r="C65" t="s">
+        <v>186</v>
+      </c>
+      <c r="D65" s="1">
         <v>43515.635416666664</v>
       </c>
-      <c r="D65">
+      <c r="E65">
         <v>-48.997904159999997</v>
       </c>
-      <c r="E65">
+      <c r="F65">
         <v>-22.764788530000001</v>
       </c>
-      <c r="F65" s="5">
+      <c r="G65" s="5">
         <v>87</v>
       </c>
-      <c r="G65" t="s">
+      <c r="H65" t="s">
         <v>158</v>
       </c>
-      <c r="H65" s="1">
+      <c r="I65" s="1">
         <v>43516.347222222219</v>
       </c>
-      <c r="I65">
+      <c r="J65">
         <v>-48.999416570000001</v>
       </c>
-      <c r="J65">
+      <c r="K65">
         <v>-22.76541568</v>
       </c>
-      <c r="K65">
+      <c r="L65">
         <v>3</v>
       </c>
-      <c r="L65">
+      <c r="M65">
         <v>168</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>72</v>
       </c>
       <c r="B66" t="s">
         <v>71</v>
       </c>
-      <c r="C66" s="1">
+      <c r="C66" t="s">
+        <v>186</v>
+      </c>
+      <c r="D66" s="1">
         <v>43515.635416666664</v>
       </c>
-      <c r="D66">
+      <c r="E66">
         <v>-48.997904159999997</v>
       </c>
-      <c r="E66">
+      <c r="F66">
         <v>-22.764788530000001</v>
       </c>
-      <c r="F66" s="5">
+      <c r="G66" s="5">
         <v>87</v>
       </c>
-      <c r="G66" t="s">
+      <c r="H66" t="s">
         <v>159</v>
       </c>
-      <c r="H66" s="1">
+      <c r="I66" s="1">
         <v>43516.350694444445</v>
       </c>
-      <c r="I66">
+      <c r="J66">
         <v>-48.999504629999997</v>
       </c>
-      <c r="J66">
+      <c r="K66">
         <v>-22.765529109999999</v>
       </c>
-      <c r="K66">
+      <c r="L66">
         <v>3</v>
       </c>
-      <c r="L66">
+      <c r="M66">
         <v>181</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>70</v>
       </c>
       <c r="B67" t="s">
         <v>73</v>
       </c>
-      <c r="C67" s="1">
+      <c r="C67" t="s">
+        <v>186</v>
+      </c>
+      <c r="D67" s="1">
         <v>43515.649305555555</v>
       </c>
-      <c r="D67">
+      <c r="E67">
         <v>-48.998105840000001</v>
       </c>
-      <c r="E67">
+      <c r="F67">
         <v>-22.76485465</v>
       </c>
-      <c r="F67" s="5">
+      <c r="G67" s="5">
         <v>88</v>
       </c>
-      <c r="G67" t="s">
+      <c r="H67" t="s">
         <v>160</v>
       </c>
-      <c r="H67" s="1">
+      <c r="I67" s="1">
         <v>43516.347222222219</v>
       </c>
-      <c r="I67">
+      <c r="J67">
         <v>-48.999416570000001</v>
       </c>
-      <c r="J67">
+      <c r="K67">
         <v>-22.76541568</v>
       </c>
-      <c r="K67">
+      <c r="L67">
         <v>3</v>
       </c>
-      <c r="L67">
+      <c r="M67">
         <v>147</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>72</v>
       </c>
       <c r="B68" t="s">
         <v>73</v>
       </c>
-      <c r="C68" s="1">
+      <c r="C68" t="s">
+        <v>186</v>
+      </c>
+      <c r="D68" s="1">
         <v>43515.649305555555</v>
       </c>
-      <c r="D68">
+      <c r="E68">
         <v>-48.998105840000001</v>
       </c>
-      <c r="E68">
+      <c r="F68">
         <v>-22.76485465</v>
       </c>
-      <c r="F68" s="5">
+      <c r="G68" s="5">
         <v>88</v>
       </c>
-      <c r="G68" t="s">
+      <c r="H68" t="s">
         <v>161</v>
       </c>
-      <c r="H68" s="1">
+      <c r="I68" s="1">
         <v>43516.350694444445</v>
       </c>
-      <c r="I68">
+      <c r="J68">
         <v>-48.999504629999997</v>
       </c>
-      <c r="J68">
+      <c r="K68">
         <v>-22.765529109999999</v>
       </c>
-      <c r="K68">
+      <c r="L68">
         <v>3</v>
       </c>
-      <c r="L68">
+      <c r="M68">
         <v>160</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>74</v>
       </c>
       <c r="B69" t="s">
         <v>64</v>
       </c>
-      <c r="C69" s="1">
+      <c r="C69" t="s">
+        <v>186</v>
+      </c>
+      <c r="D69" s="1">
         <v>43516.350694444445</v>
       </c>
-      <c r="D69">
+      <c r="E69">
         <v>-48.999504629999997</v>
       </c>
-      <c r="E69">
+      <c r="F69">
         <v>-22.765529109999999</v>
       </c>
-      <c r="F69" s="5">
+      <c r="G69" s="5">
         <v>89</v>
       </c>
-      <c r="G69" t="s">
+      <c r="H69" t="s">
         <v>162</v>
       </c>
-      <c r="H69" s="1">
+      <c r="I69" s="1">
         <v>43516.4375</v>
       </c>
-      <c r="I69">
+      <c r="J69">
         <v>-49.00003976</v>
       </c>
-      <c r="J69">
+      <c r="K69">
         <v>-22.76571306</v>
       </c>
-      <c r="K69">
+      <c r="L69">
         <v>3</v>
       </c>
-      <c r="L69">
+      <c r="M69">
         <v>58</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>74</v>
       </c>
       <c r="B70" t="s">
         <v>66</v>
       </c>
-      <c r="C70" s="1">
+      <c r="C70" t="s">
+        <v>186</v>
+      </c>
+      <c r="D70" s="1">
         <v>43516.361111111109</v>
       </c>
-      <c r="D70">
+      <c r="E70">
         <v>-48.999521590000001</v>
       </c>
-      <c r="E70">
+      <c r="F70">
         <v>-22.765641930000001</v>
       </c>
-      <c r="F70" s="5">
+      <c r="G70" s="5">
         <v>90</v>
       </c>
-      <c r="G70" t="s">
+      <c r="H70" t="s">
         <v>163</v>
       </c>
-      <c r="H70" s="1">
+      <c r="I70" s="1">
         <v>43516.4375</v>
       </c>
-      <c r="I70">
+      <c r="J70">
         <v>-49.00003976</v>
       </c>
-      <c r="J70">
+      <c r="K70">
         <v>-22.76571306</v>
       </c>
-      <c r="K70">
+      <c r="L70">
         <v>2</v>
       </c>
-      <c r="L70">
+      <c r="M70">
         <v>54</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>75</v>
       </c>
       <c r="B71" t="s">
         <v>76</v>
       </c>
-      <c r="C71" s="1">
+      <c r="C71" t="s">
+        <v>186</v>
+      </c>
+      <c r="D71" s="1">
         <v>43516.444444444445</v>
       </c>
-      <c r="D71">
+      <c r="E71">
         <v>-49.000087669999999</v>
       </c>
-      <c r="E71">
+      <c r="F71">
         <v>-22.76564093</v>
       </c>
-      <c r="F71" s="5">
+      <c r="G71" s="5">
         <v>93</v>
       </c>
-      <c r="G71" t="s">
+      <c r="H71" t="s">
         <v>164</v>
       </c>
-      <c r="H71" s="1">
+      <c r="I71" s="1">
         <v>43516.472222222219</v>
       </c>
-      <c r="I71">
+      <c r="J71">
         <v>-48.999708660000003</v>
       </c>
-      <c r="J71">
+      <c r="K71">
         <v>-22.764785310000001</v>
       </c>
-      <c r="K71" t="s">
+      <c r="L71" t="s">
         <v>29</v>
       </c>
-      <c r="L71">
+      <c r="M71">
         <v>96</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>77</v>
       </c>
       <c r="B72" t="s">
         <v>73</v>
       </c>
-      <c r="C72" s="1">
+      <c r="C72" t="s">
+        <v>186</v>
+      </c>
+      <c r="D72" s="1">
         <v>43516.590277777781</v>
       </c>
-      <c r="D72">
+      <c r="E72">
         <v>-48.999215640000003</v>
       </c>
-      <c r="E72">
+      <c r="F72">
         <v>-22.76468504</v>
       </c>
-      <c r="F72" s="5">
+      <c r="G72" s="5">
         <v>95</v>
       </c>
-      <c r="G72" t="s">
+      <c r="H72" t="s">
         <v>165</v>
       </c>
-      <c r="H72" s="1">
+      <c r="I72" s="1">
         <v>43516.708333333336</v>
       </c>
-      <c r="I72">
+      <c r="J72">
         <v>-48.996641400000001</v>
       </c>
-      <c r="J72">
+      <c r="K72">
         <v>-22.764263369999998</v>
       </c>
-      <c r="K72">
+      <c r="L72">
         <v>3</v>
       </c>
-      <c r="L72">
+      <c r="M72">
         <v>269</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>77</v>
       </c>
       <c r="B73" t="s">
         <v>64</v>
       </c>
-      <c r="C73" s="1">
+      <c r="C73" t="s">
+        <v>186</v>
+      </c>
+      <c r="D73" s="1">
         <v>43516.618055555555</v>
       </c>
-      <c r="D73">
+      <c r="E73">
         <v>-48.998619840000003</v>
       </c>
-      <c r="E73">
+      <c r="F73">
         <v>-22.764437900000001</v>
       </c>
-      <c r="F73" s="5">
+      <c r="G73" s="5">
         <v>96</v>
       </c>
-      <c r="G73" t="s">
+      <c r="H73" t="s">
         <v>166</v>
       </c>
-      <c r="H73" s="1">
+      <c r="I73" s="1">
         <v>43516.708333333336</v>
       </c>
-      <c r="I73">
+      <c r="J73">
         <v>-48.996641400000001</v>
       </c>
-      <c r="J73">
+      <c r="K73">
         <v>-22.764263369999998</v>
       </c>
-      <c r="K73">
+      <c r="L73">
         <v>4</v>
       </c>
-      <c r="L73">
+      <c r="M73">
         <v>204</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>78</v>
       </c>
       <c r="B74" t="s">
         <v>13</v>
       </c>
-      <c r="C74" s="1">
+      <c r="C74" t="s">
+        <v>186</v>
+      </c>
+      <c r="D74" s="1">
         <v>43517.381944444445</v>
       </c>
-      <c r="D74">
+      <c r="E74">
         <v>-48.996229530000001</v>
       </c>
-      <c r="E74">
+      <c r="F74">
         <v>-22.76405462</v>
       </c>
-      <c r="F74" s="5">
+      <c r="G74" s="5">
         <v>99</v>
       </c>
-      <c r="G74" t="s">
+      <c r="H74" t="s">
         <v>167</v>
       </c>
-      <c r="H74" s="1">
+      <c r="I74" s="1">
         <v>43517.611111111109</v>
       </c>
-      <c r="I74">
+      <c r="J74">
         <v>-48.993713120000002</v>
       </c>
-      <c r="J74">
+      <c r="K74">
         <v>-22.761366550000002</v>
       </c>
-      <c r="K74">
+      <c r="L74">
         <v>5</v>
       </c>
-      <c r="L74">
+      <c r="M74">
         <v>378</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>79</v>
       </c>
       <c r="B75" t="s">
         <v>80</v>
       </c>
-      <c r="C75" s="1">
+      <c r="C75" t="s">
+        <v>186</v>
+      </c>
+      <c r="D75" s="1">
         <v>43517.489583333336</v>
       </c>
-      <c r="D75">
+      <c r="E75">
         <v>-48.995236630000001</v>
       </c>
-      <c r="E75">
+      <c r="F75">
         <v>-22.76223912</v>
       </c>
-      <c r="F75" s="5">
+      <c r="G75" s="5">
         <v>100</v>
       </c>
-      <c r="G75" t="s">
+      <c r="H75" t="s">
         <v>168</v>
       </c>
-      <c r="H75" s="1">
+      <c r="I75" s="1">
         <v>43517.621527777781</v>
       </c>
-      <c r="I75">
+      <c r="J75">
         <v>-48.993211109999997</v>
       </c>
-      <c r="J75">
+      <c r="K75">
         <v>-22.761829209999998</v>
       </c>
-      <c r="K75">
+      <c r="L75">
         <v>2</v>
       </c>
-      <c r="L75">
+      <c r="M75">
         <v>213</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>79</v>
       </c>
       <c r="B76" t="s">
         <v>64</v>
       </c>
-      <c r="C76" s="1">
+      <c r="C76" t="s">
+        <v>186</v>
+      </c>
+      <c r="D76" s="1">
         <v>43517.503472222219</v>
       </c>
-      <c r="D76">
+      <c r="E76">
         <v>-48.99495494</v>
       </c>
-      <c r="E76">
+      <c r="F76">
         <v>-22.761945279999999</v>
       </c>
-      <c r="F76" s="5">
+      <c r="G76" s="5">
         <v>101</v>
       </c>
-      <c r="G76" t="s">
+      <c r="H76" t="s">
         <v>169</v>
       </c>
-      <c r="H76" s="1">
+      <c r="I76" s="1">
         <v>43517.621527777781</v>
       </c>
-      <c r="I76">
+      <c r="J76">
         <v>-48.993211109999997</v>
       </c>
-      <c r="J76">
+      <c r="K76">
         <v>-22.761829209999998</v>
       </c>
-      <c r="K76">
+      <c r="L76">
         <v>5</v>
       </c>
-      <c r="L76">
+      <c r="M76">
         <v>180</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>81</v>
       </c>
       <c r="B77" t="s">
         <v>76</v>
       </c>
-      <c r="C77" s="1">
+      <c r="C77" t="s">
+        <v>186</v>
+      </c>
+      <c r="D77" s="1">
         <v>43518.375</v>
       </c>
-      <c r="D77">
+      <c r="E77">
         <v>-48.993160830000001</v>
       </c>
-      <c r="E77">
+      <c r="F77">
         <v>-22.763850170000001</v>
       </c>
-      <c r="F77" s="5">
+      <c r="G77" s="5">
         <v>105</v>
       </c>
-      <c r="G77" t="s">
+      <c r="H77" t="s">
         <v>170</v>
       </c>
-      <c r="H77" s="1">
+      <c r="I77" s="1">
         <v>43518.416666666664</v>
       </c>
-      <c r="I77">
+      <c r="J77">
         <v>-48.99355911</v>
       </c>
-      <c r="J77">
+      <c r="K77">
         <v>-22.764021499999998</v>
       </c>
-      <c r="K77" t="s">
+      <c r="L77" t="s">
         <v>29</v>
       </c>
-      <c r="L77">
+      <c r="M77">
         <v>45</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>82</v>
       </c>
       <c r="B78" t="s">
         <v>80</v>
       </c>
-      <c r="C78" s="1">
+      <c r="C78" t="s">
+        <v>186</v>
+      </c>
+      <c r="D78" s="1">
         <v>43518.59375</v>
       </c>
-      <c r="D78">
+      <c r="E78">
         <v>-48.994137729999998</v>
       </c>
-      <c r="E78">
+      <c r="F78">
         <v>-22.761754700000001</v>
       </c>
-      <c r="F78" s="5">
+      <c r="G78" s="5">
         <v>108</v>
       </c>
-      <c r="G78" t="s">
+      <c r="H78" t="s">
         <v>171</v>
       </c>
-      <c r="H78" s="1">
+      <c r="I78" s="1">
         <v>43518.715277777781</v>
       </c>
-      <c r="I78">
+      <c r="J78">
         <v>-48.995849300000003</v>
       </c>
-      <c r="J78">
+      <c r="K78">
         <v>-22.76101027</v>
       </c>
-      <c r="K78">
+      <c r="L78">
         <v>1</v>
       </c>
-      <c r="L78">
+      <c r="M78">
         <v>192</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>82</v>
       </c>
       <c r="B79" t="s">
         <v>13</v>
       </c>
-      <c r="C79" s="1">
+      <c r="C79" t="s">
+        <v>186</v>
+      </c>
+      <c r="D79" s="1">
         <v>43518.638888888891</v>
       </c>
-      <c r="D79">
+      <c r="E79">
         <v>-48.994181480000002</v>
       </c>
-      <c r="E79">
+      <c r="F79">
         <v>-22.761079680000002</v>
       </c>
-      <c r="F79" s="5">
+      <c r="G79" s="5">
         <v>110</v>
       </c>
-      <c r="G79" t="s">
+      <c r="H79" t="s">
         <v>172</v>
       </c>
-      <c r="H79" s="1">
+      <c r="I79" s="1">
         <v>43518.715277777781</v>
       </c>
-      <c r="I79">
+      <c r="J79">
         <v>-48.995849300000003</v>
       </c>
-      <c r="J79">
+      <c r="K79">
         <v>-22.76101027</v>
       </c>
-      <c r="K79">
+      <c r="L79">
         <v>5</v>
       </c>
-      <c r="L79">
+      <c r="M79">
         <v>172</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>83</v>
       </c>
       <c r="B80" t="s">
         <v>84</v>
       </c>
-      <c r="C80" s="1">
+      <c r="C80" t="s">
+        <v>187</v>
+      </c>
+      <c r="D80" s="1">
         <v>43561.527777777781</v>
       </c>
-      <c r="D80">
+      <c r="E80">
         <v>-48.996477810000002</v>
       </c>
-      <c r="E80">
+      <c r="F80">
         <v>-22.762497029999999</v>
       </c>
-      <c r="F80" s="5">
+      <c r="G80" s="5">
         <v>112</v>
       </c>
-      <c r="G80" t="s">
+      <c r="H80" t="s">
         <v>173</v>
       </c>
-      <c r="H80" s="1">
+      <c r="I80" s="1">
         <v>43561.618055555555</v>
       </c>
-      <c r="I80">
+      <c r="J80">
         <v>-48.994985200000002</v>
       </c>
-      <c r="J80">
+      <c r="K80">
         <v>-22.760821570000001</v>
       </c>
-      <c r="K80">
+      <c r="L80">
         <v>4</v>
       </c>
-      <c r="L80">
+      <c r="M80">
         <v>231</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>85</v>
       </c>
       <c r="B81" t="s">
         <v>84</v>
       </c>
-      <c r="C81" s="1">
+      <c r="C81" t="s">
+        <v>187</v>
+      </c>
+      <c r="D81" s="1">
         <v>43561.670138888891</v>
       </c>
-      <c r="D81">
+      <c r="E81">
         <v>-48.99389429</v>
       </c>
-      <c r="E81">
+      <c r="F81">
         <v>-22.76195753</v>
       </c>
-      <c r="F81" s="5">
+      <c r="G81" s="5">
         <v>114</v>
       </c>
-      <c r="G81" t="s">
+      <c r="H81" t="s">
         <v>174</v>
       </c>
-      <c r="H81" s="1">
+      <c r="I81" s="1">
         <v>43562.388888888891</v>
       </c>
-      <c r="I81">
+      <c r="J81">
         <v>-48.995618530000002</v>
       </c>
-      <c r="J81">
+      <c r="K81">
         <v>-22.762099979999999</v>
       </c>
-      <c r="K81">
+      <c r="L81">
         <v>4</v>
       </c>
-      <c r="L81">
+      <c r="M81">
         <v>178</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>86</v>
       </c>
       <c r="B82" t="s">
         <v>87</v>
       </c>
-      <c r="C82" s="1">
+      <c r="C82" t="s">
+        <v>187</v>
+      </c>
+      <c r="D82" s="1">
         <v>43562.604166666664</v>
       </c>
-      <c r="D82">
+      <c r="E82">
         <v>-48.994640189999998</v>
       </c>
-      <c r="E82">
+      <c r="F82">
         <v>-22.762430219999999</v>
       </c>
-      <c r="F82" s="5">
+      <c r="G82" s="5">
         <v>119</v>
       </c>
-      <c r="G82" t="s">
+      <c r="H82" t="s">
         <v>175</v>
       </c>
-      <c r="H82" s="1">
+      <c r="I82" s="1">
         <v>43563.340277777781</v>
       </c>
-      <c r="I82">
+      <c r="J82">
         <v>-48.993108370000002</v>
       </c>
-      <c r="J82">
+      <c r="K82">
         <v>-22.762153479999998</v>
       </c>
-      <c r="K82">
+      <c r="L82">
         <v>6</v>
       </c>
-      <c r="L82">
+      <c r="M82">
         <v>160</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>86</v>
       </c>
       <c r="B83" t="s">
         <v>88</v>
       </c>
-      <c r="C83" s="1">
+      <c r="C83" t="s">
+        <v>187</v>
+      </c>
+      <c r="D83" s="1">
         <v>43562.670138888891</v>
       </c>
-      <c r="D83">
+      <c r="E83">
         <v>-48.993818869999998</v>
       </c>
-      <c r="E83">
+      <c r="F83">
         <v>-22.761850339999999</v>
       </c>
-      <c r="F83" s="5">
+      <c r="G83" s="5">
         <v>120</v>
       </c>
-      <c r="G83" t="s">
+      <c r="H83" t="s">
         <v>176</v>
       </c>
-      <c r="H83" s="1">
+      <c r="I83" s="1">
         <v>43563.340277777781</v>
       </c>
-      <c r="I83">
+      <c r="J83">
         <v>-48.993108370000002</v>
       </c>
-      <c r="J83">
+      <c r="K83">
         <v>-22.762153479999998</v>
       </c>
-      <c r="K83" t="s">
+      <c r="L83" t="s">
         <v>29</v>
       </c>
-      <c r="L83">
+      <c r="M83">
         <v>79</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>89</v>
       </c>
       <c r="B84" t="s">
         <v>87</v>
       </c>
-      <c r="C84" s="1">
+      <c r="C84" t="s">
+        <v>187</v>
+      </c>
+      <c r="D84" s="1">
         <v>43564.496527777781</v>
       </c>
-      <c r="D84">
+      <c r="E84">
         <v>-48.995843809999997</v>
       </c>
-      <c r="E84">
+      <c r="F84">
         <v>-22.763871949999999</v>
       </c>
-      <c r="F84" s="5">
+      <c r="G84" s="5">
         <v>126</v>
       </c>
-      <c r="G84" t="s">
+      <c r="H84" t="s">
         <v>177</v>
       </c>
-      <c r="H84" s="1">
+      <c r="I84" s="1">
         <v>43564.576388888891</v>
       </c>
-      <c r="I84">
+      <c r="J84">
         <v>-48.996098879999998</v>
       </c>
-      <c r="J84">
+      <c r="K84">
         <v>-22.762305260000002</v>
       </c>
-      <c r="K84">
+      <c r="L84">
         <v>7</v>
       </c>
-      <c r="L84">
+      <c r="M84">
         <v>163</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>90</v>
       </c>
       <c r="B85" t="s">
         <v>88</v>
       </c>
-      <c r="C85" s="1">
+      <c r="C85" t="s">
+        <v>187</v>
+      </c>
+      <c r="D85" s="1">
         <v>43564.565972222219</v>
       </c>
-      <c r="D85">
+      <c r="E85">
         <v>-48.996109390000001</v>
       </c>
-      <c r="E85">
+      <c r="F85">
         <v>-22.762440120000001</v>
       </c>
-      <c r="F85" s="5">
+      <c r="G85" s="5">
         <v>127</v>
       </c>
-      <c r="G85" t="s">
+      <c r="H85" t="s">
         <v>178</v>
       </c>
-      <c r="H85" s="1">
+      <c r="I85" s="1">
         <v>43564.680555555555</v>
       </c>
-      <c r="I85">
+      <c r="J85">
         <v>-48.994567439999997</v>
       </c>
-      <c r="J85">
+      <c r="K85">
         <v>-22.761506239999999</v>
       </c>
-      <c r="K85" t="s">
+      <c r="L85" t="s">
         <v>29</v>
       </c>
-      <c r="L85">
+      <c r="M85">
         <v>185</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>90</v>
       </c>
       <c r="B86" t="s">
         <v>87</v>
       </c>
-      <c r="C86" s="1">
+      <c r="C86" t="s">
+        <v>187</v>
+      </c>
+      <c r="D86" s="1">
         <v>43564.59375</v>
       </c>
-      <c r="D86">
+      <c r="E86">
         <v>-48.996178299999997</v>
       </c>
-      <c r="E86">
+      <c r="F86">
         <v>-22.762265240000001</v>
       </c>
-      <c r="F86" s="5">
+      <c r="G86" s="5">
         <v>128</v>
       </c>
-      <c r="G86" t="s">
+      <c r="H86" t="s">
         <v>179</v>
       </c>
-      <c r="H86" s="1">
+      <c r="I86" s="1">
         <v>43564.680555555555</v>
       </c>
-      <c r="I86">
+      <c r="J86">
         <v>-48.994567439999997</v>
       </c>
-      <c r="J86">
+      <c r="K86">
         <v>-22.761506239999999</v>
       </c>
-      <c r="K86">
+      <c r="L86">
         <v>6</v>
       </c>
-      <c r="L86">
+      <c r="M86">
         <v>183</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>91</v>
       </c>
       <c r="B87" t="s">
         <v>92</v>
       </c>
-      <c r="C87" s="1">
+      <c r="C87" t="s">
+        <v>187</v>
+      </c>
+      <c r="D87" s="1">
         <v>43568.631944444445</v>
       </c>
-      <c r="D87">
+      <c r="E87">
         <v>-48.997669709999997</v>
       </c>
-      <c r="E87">
+      <c r="F87">
         <v>-22.76414737</v>
       </c>
-      <c r="F87" s="5">
+      <c r="G87" s="5">
         <v>134</v>
       </c>
-      <c r="G87" t="s">
+      <c r="H87" t="s">
         <v>180</v>
       </c>
-      <c r="H87" s="1">
+      <c r="I87" s="1">
         <v>43568.697916666664</v>
       </c>
-      <c r="I87">
+      <c r="J87">
         <v>-48.99638856</v>
       </c>
-      <c r="J87">
+      <c r="K87">
         <v>-22.7645056</v>
       </c>
-      <c r="K87">
+      <c r="L87">
         <v>2</v>
       </c>
-      <c r="L87">
+      <c r="M87">
         <v>137</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>91</v>
       </c>
       <c r="B88" t="s">
         <v>93</v>
       </c>
-      <c r="C88" s="1">
+      <c r="C88" t="s">
+        <v>187</v>
+      </c>
+      <c r="D88" s="1">
         <v>43568.631944444445</v>
       </c>
-      <c r="D88">
+      <c r="E88">
         <v>-48.997669709999997</v>
       </c>
-      <c r="E88">
+      <c r="F88">
         <v>-22.76414737</v>
       </c>
-      <c r="F88" s="5">
+      <c r="G88" s="5">
         <v>135</v>
       </c>
-      <c r="G88" t="s">
+      <c r="H88" t="s">
         <v>181</v>
       </c>
-      <c r="H88" s="1">
+      <c r="I88" s="1">
         <v>43568.697916666664</v>
       </c>
-      <c r="I88">
+      <c r="J88">
         <v>-48.99638856</v>
       </c>
-      <c r="J88">
+      <c r="K88">
         <v>-22.7645056</v>
       </c>
-      <c r="K88">
+      <c r="L88">
         <v>7</v>
       </c>
-      <c r="L88">
+      <c r="M88">
         <v>137</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>94</v>
       </c>
       <c r="B89" t="s">
         <v>88</v>
       </c>
-      <c r="C89" s="1">
+      <c r="C89" t="s">
+        <v>187</v>
+      </c>
+      <c r="D89" s="1">
         <v>43569.347222222219</v>
       </c>
-      <c r="D89">
+      <c r="E89">
         <v>-48.9968918</v>
       </c>
-      <c r="E89">
+      <c r="F89">
         <v>-22.764352250000002</v>
       </c>
-      <c r="F89" s="5">
+      <c r="G89" s="5">
         <v>136</v>
       </c>
-      <c r="G89" t="s">
+      <c r="H89" t="s">
         <v>182</v>
       </c>
-      <c r="H89" s="1">
+      <c r="I89" s="1">
         <v>43569.402777777781</v>
       </c>
-      <c r="I89">
+      <c r="J89">
         <v>-48.996458279999999</v>
       </c>
-      <c r="J89">
+      <c r="K89">
         <v>-22.763005379999999</v>
       </c>
-      <c r="K89" t="s">
+      <c r="L89" t="s">
         <v>29</v>
       </c>
-      <c r="L89">
+      <c r="M89">
         <v>145</v>
       </c>
     </row>

</xml_diff>